<commit_message>
Add data for Tungsten
</commit_message>
<xml_diff>
--- a/Jupyter/Tungsten/Tungsten.xlsx
+++ b/Jupyter/Tungsten/Tungsten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuqih\Documents\GitHub\DatabaseCodes\Jupyter\Tungsten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FC70C4-7941-4469-92A7-D4B58AAB9872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6874656-150C-4A84-8E65-9FE7D756A8B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="852" activeTab="10" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="852" firstSheet="1" activeTab="3" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
   </bookViews>
   <sheets>
     <sheet name="W_density" sheetId="15" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="90">
   <si>
     <t>W-Fujitsuka</t>
   </si>
@@ -420,6 +420,39 @@
   </si>
   <si>
     <t>Total Elongation (%)</t>
+  </si>
+  <si>
+    <t>W HR-EP</t>
+  </si>
+  <si>
+    <t>W HR-AM</t>
+  </si>
+  <si>
+    <t>W Forge</t>
+  </si>
+  <si>
+    <t>W Pure</t>
+  </si>
+  <si>
+    <t>W 1%Re</t>
+  </si>
+  <si>
+    <t>W 3%Re</t>
+  </si>
+  <si>
+    <t>W K-doped 3%Re</t>
+  </si>
+  <si>
+    <t>W K-doped Rod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W K-doped </t>
+  </si>
+  <si>
+    <t>Thermal Conductivity (W/m k)</t>
+  </si>
+  <si>
+    <t>Nogami2021-- Mechanical properties of tungsten-Recent research on modified tungsten materials in Japan</t>
   </si>
 </sst>
 </file>
@@ -512,7 +545,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -550,6 +583,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -624,12 +660,105 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>440121</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B70BE93-8661-7F52-05BA-AD3C162A35EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3619501"/>
+          <a:ext cx="4745421" cy="2457450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>229208</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>362379</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{134AE577-4DCF-DC60-81AD-8570DD8E4761}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5438775" y="4267200"/>
+          <a:ext cx="4353533" cy="3077004"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>21003</xdr:rowOff>
     </xdr:to>
@@ -664,10 +793,54 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>638783</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>390954</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9043AE5B-A2A4-EF63-6520-4AB61247D691}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6267450" y="4171950"/>
+          <a:ext cx="4353533" cy="3077004"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -716,7 +889,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -765,7 +938,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -858,7 +1031,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1006,6 +1179,55 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>172008</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>57637</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAB4C43D-9087-3E1F-D6BC-020C930E1A60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3619500"/>
+          <a:ext cx="4001058" cy="3486637"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1049,7 +1271,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1098,7 +1320,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1147,7 +1369,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1196,7 +1418,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -1240,7 +1462,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1278,55 +1500,6 @@
         <a:xfrm>
           <a:off x="104775" y="3190875"/>
           <a:ext cx="4152900" cy="3284779"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>478221</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B70BE93-8661-7F52-05BA-AD3C162A35EC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="3619501"/>
-          <a:ext cx="4745421" cy="2457450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1676,7 +1849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E49AD77F-8B12-49E9-AB0E-8DA6E26FE1AE}">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
@@ -2795,8 +2968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689ABF1C-EFBF-442E-A0BE-50F31494446C}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3039,15 +3212,27 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3020762B-09A6-4698-8DE0-2E0869AA4EBF}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37:I38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.85546875" customWidth="1"/>
+    <col min="4" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" customWidth="1"/>
+    <col min="7" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="4.85546875" customWidth="1"/>
+    <col min="13" max="14" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>20</v>
       </c>
@@ -3057,8 +3242,20 @@
         <v>75</v>
       </c>
       <c r="E1" s="12"/>
-    </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="G1" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="J1" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1" s="14"/>
+      <c r="M1" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="14"/>
+    </row>
+    <row r="3" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -3071,8 +3268,26 @@
       <c r="E3" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>356.24990316799199</v>
       </c>
@@ -3085,8 +3300,26 @@
       <c r="E4">
         <v>19.1643911413667</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>298.430898876404</v>
+      </c>
+      <c r="H4">
+        <v>0.116732826481865</v>
+      </c>
+      <c r="J4">
+        <v>297.30730337078597</v>
+      </c>
+      <c r="K4">
+        <v>0.176747628338837</v>
+      </c>
+      <c r="M4">
+        <v>422.58820224719102</v>
+      </c>
+      <c r="N4">
+        <v>1.4192289578146999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>464.34949290898402</v>
       </c>
@@ -3099,8 +3332,26 @@
       <c r="E5">
         <v>6.3145556845843798</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>422.58820224719102</v>
+      </c>
+      <c r="H5">
+        <v>0.16174392787459599</v>
+      </c>
+      <c r="J5">
+        <v>473.71179775280802</v>
+      </c>
+      <c r="K5">
+        <v>2.19154948529907</v>
+      </c>
+      <c r="M5">
+        <v>423.15</v>
+      </c>
+      <c r="N5">
+        <v>0.28143712574850999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>568.54186856295303</v>
       </c>
@@ -3113,8 +3364,26 @@
       <c r="E6">
         <v>14.9251120247103</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>472.58820224719</v>
+      </c>
+      <c r="H6">
+        <v>9.5875664401532307E-2</v>
+      </c>
+      <c r="J6">
+        <v>472.58820224719</v>
+      </c>
+      <c r="K6">
+        <v>3.3892888380542199</v>
+      </c>
+      <c r="M6">
+        <v>472.58820224719</v>
+      </c>
+      <c r="N6">
+        <v>1.17371997577878</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>657.10538786882603</v>
       </c>
@@ -3127,8 +3396,26 @@
       <c r="E7">
         <v>21.0978834566763</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>523.15</v>
+      </c>
+      <c r="H7">
+        <v>11.6467065868263</v>
+      </c>
+      <c r="J7">
+        <v>522.58820224719102</v>
+      </c>
+      <c r="K7">
+        <v>13.1437798560183</v>
+      </c>
+      <c r="M7">
+        <v>523.15</v>
+      </c>
+      <c r="N7">
+        <v>2.9940119760482199E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>762.60016821846796</v>
       </c>
@@ -3141,8 +3428,26 @@
       <c r="E8">
         <v>15.086792448395199</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>573.15</v>
+      </c>
+      <c r="H8">
+        <v>18.766467065868198</v>
+      </c>
+      <c r="J8">
+        <v>571.46460674157197</v>
+      </c>
+      <c r="K8">
+        <v>31.101998250689601</v>
+      </c>
+      <c r="M8">
+        <v>523.71179775280802</v>
+      </c>
+      <c r="N8">
+        <v>1.6466393056583499</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>862.88532978541298</v>
       </c>
@@ -3155,8 +3460,26 @@
       <c r="E9">
         <v>16.385144541439701</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>623.71179775280802</v>
+      </c>
+      <c r="H9">
+        <v>29.658615353562499</v>
+      </c>
+      <c r="J9">
+        <v>572.02640449438195</v>
+      </c>
+      <c r="K9">
+        <v>34.095942945569497</v>
+      </c>
+      <c r="M9">
+        <v>573.15</v>
+      </c>
+      <c r="N9">
+        <v>0.56287425149700698</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1165.04321918192</v>
       </c>
@@ -3169,8 +3492,26 @@
       <c r="E10">
         <v>11.310388738256</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>673.71179775280802</v>
+      </c>
+      <c r="H10">
+        <v>29.5927470900894</v>
+      </c>
+      <c r="J10">
+        <v>622.58820224719102</v>
+      </c>
+      <c r="K10">
+        <v>31.275516382964401</v>
+      </c>
+      <c r="M10">
+        <v>573.71179775280802</v>
+      </c>
+      <c r="N10">
+        <v>3.9759806230236099</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1372.1255657941799</v>
       </c>
@@ -3183,8 +3524,26 @@
       <c r="E11">
         <v>11.2968131049579</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>722.58820224719102</v>
+      </c>
+      <c r="H11">
+        <v>35.6347978200901</v>
+      </c>
+      <c r="J11">
+        <v>622.58820224719102</v>
+      </c>
+      <c r="K11">
+        <v>28.7605463230841</v>
+      </c>
+      <c r="M11">
+        <v>623.71179775280802</v>
+      </c>
+      <c r="N11">
+        <v>5.2873578685325997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1562.27665136268</v>
       </c>
@@ -3197,24 +3556,130 @@
       <c r="E12">
         <v>13.145323489791799</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>774.27359550561698</v>
+      </c>
+      <c r="H12">
+        <v>36.227410347843602</v>
+      </c>
+      <c r="J12">
+        <v>623.14999999999895</v>
+      </c>
+      <c r="K12">
+        <v>25.4071856287425</v>
+      </c>
+      <c r="M12">
+        <v>623.71179775280802</v>
+      </c>
+      <c r="N12">
+        <v>13.6107111619457</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D13">
         <v>1288.7110551722601</v>
       </c>
       <c r="E13">
         <v>15.0882497197661</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>672.58820224719102</v>
+      </c>
+      <c r="K13">
+        <v>31.808450514700901</v>
+      </c>
+      <c r="M13">
+        <v>673.15</v>
+      </c>
+      <c r="N13">
+        <v>14.682634730538901</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>1478.74622358397</v>
       </c>
       <c r="E14">
         <v>23.122186787945601</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>672.58820224719102</v>
+      </c>
+      <c r="K14">
+        <v>30.311444526676901</v>
+      </c>
+      <c r="M14">
+        <v>723.15</v>
+      </c>
+      <c r="N14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>723.15</v>
+      </c>
+      <c r="K15">
+        <v>29.706586826347301</v>
+      </c>
+      <c r="M15">
+        <v>722.58820224719102</v>
+      </c>
+      <c r="N15">
+        <v>16.4731211733835</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>722.02640449438195</v>
+      </c>
+      <c r="K16">
+        <v>27.431272286886902</v>
+      </c>
+      <c r="M16">
+        <v>774.83539325842605</v>
+      </c>
+      <c r="N16">
+        <v>17.544708336136701</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>772.02640449438195</v>
+      </c>
+      <c r="K17">
+        <v>32.5749848617372</v>
+      </c>
+      <c r="M17">
+        <v>773.71179775280802</v>
+      </c>
+      <c r="N17">
+        <v>23.413106371526599</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>772.58820224719</v>
+      </c>
+      <c r="K18">
+        <v>31.856354706317699</v>
+      </c>
+      <c r="M18">
+        <v>724.27359550561698</v>
+      </c>
+      <c r="N18">
+        <v>22.5208235214963</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>672.58820224719102</v>
+      </c>
+      <c r="N19">
+        <v>22.467133149431401</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>76</v>
       </c>
@@ -3233,11 +3698,14 @@
       <c r="E33" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="M1:N1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A33:E33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3246,18 +3714,27 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4DEC4A-2FB4-4F74-97C1-3931F806A241}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:E36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="2" width="16.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="4" style="2" customWidth="1"/>
+    <col min="4" max="5" width="16.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="4" style="2" customWidth="1"/>
+    <col min="7" max="8" width="16.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="4" style="2" customWidth="1"/>
+    <col min="10" max="11" width="16.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="4" style="2" customWidth="1"/>
+    <col min="13" max="14" width="16.7109375" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>20</v>
       </c>
@@ -3266,8 +3743,22 @@
         <v>75</v>
       </c>
       <c r="E1" s="12"/>
-    </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="G1" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1"/>
+      <c r="J1" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1" s="14"/>
+      <c r="L1"/>
+      <c r="M1" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="14"/>
+    </row>
+    <row r="3" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -3280,8 +3771,26 @@
       <c r="E3" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>367.83559215159102</v>
       </c>
@@ -3294,8 +3803,26 @@
       <c r="E4" s="2">
         <v>13.9244105734671</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>523.15</v>
+      </c>
+      <c r="H4">
+        <v>6.5568862275449096</v>
+      </c>
+      <c r="J4">
+        <v>523.15</v>
+      </c>
+      <c r="K4">
+        <v>6.2574850299401197</v>
+      </c>
+      <c r="M4">
+        <v>522.58820224719102</v>
+      </c>
+      <c r="N4">
+        <v>1.40725290991051</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>472.52664297066599</v>
       </c>
@@ -3308,8 +3835,26 @@
       <c r="E5" s="2">
         <v>7.2539846854706402</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>573.15</v>
+      </c>
+      <c r="H5">
+        <v>6.6706586826347296</v>
+      </c>
+      <c r="J5">
+        <v>473.15</v>
+      </c>
+      <c r="K5">
+        <v>2.1317365269461002</v>
+      </c>
+      <c r="M5">
+        <v>573.15</v>
+      </c>
+      <c r="N5">
+        <v>3.4371257485029898</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>566.722526480841</v>
       </c>
@@ -3322,8 +3867,26 @@
       <c r="E6" s="2">
         <v>10.6545939617041</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>623.14999999999895</v>
+      </c>
+      <c r="H6">
+        <v>9.7784431137724592</v>
+      </c>
+      <c r="J6">
+        <v>572.58820224719102</v>
+      </c>
+      <c r="K6">
+        <v>7.8084505147009304</v>
+      </c>
+      <c r="M6">
+        <v>623.14999999999895</v>
+      </c>
+      <c r="N6">
+        <v>2.6526946107784402</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>677.66211737605204</v>
       </c>
@@ -3336,8 +3899,26 @@
       <c r="E7" s="2">
         <v>8.4747162205287996</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>673.15</v>
+      </c>
+      <c r="H7">
+        <v>8.2155688622754504</v>
+      </c>
+      <c r="J7">
+        <v>623.14999999999895</v>
+      </c>
+      <c r="K7">
+        <v>6.60479041916168</v>
+      </c>
+      <c r="M7">
+        <v>623.14999999999895</v>
+      </c>
+      <c r="N7">
+        <v>4.0898203592814397</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>767.52730195348499</v>
       </c>
@@ -3350,8 +3931,26 @@
       <c r="E8" s="2">
         <v>4.59453384123674</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>722.58820224719102</v>
+      </c>
+      <c r="H8">
+        <v>6.3533606943416601</v>
+      </c>
+      <c r="J8">
+        <v>623.14999999999895</v>
+      </c>
+      <c r="K8">
+        <v>5.52694610778443</v>
+      </c>
+      <c r="M8">
+        <v>673.15</v>
+      </c>
+      <c r="N8">
+        <v>3.8443113772455102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>861.25238394378698</v>
       </c>
@@ -3364,8 +3963,26 @@
       <c r="E9" s="2">
         <v>6.1204482600594696</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>773.71179775280802</v>
+      </c>
+      <c r="H9">
+        <v>5.1496333176343896</v>
+      </c>
+      <c r="J9">
+        <v>672.02640449438195</v>
+      </c>
+      <c r="K9">
+        <v>5.4013321671264203</v>
+      </c>
+      <c r="M9">
+        <v>673.15</v>
+      </c>
+      <c r="N9">
+        <v>3.12574850299402</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>975.78284281193999</v>
       </c>
@@ -3378,8 +3995,20 @@
       <c r="E10" s="2">
         <v>3.0250218675905298</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>722.58820224719102</v>
+      </c>
+      <c r="K10">
+        <v>6.3533606943416601</v>
+      </c>
+      <c r="M10">
+        <v>723.15</v>
+      </c>
+      <c r="N10">
+        <v>4.2574850299401197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1178.9715541708999</v>
       </c>
@@ -3392,8 +4021,20 @@
       <c r="E11" s="2">
         <v>2.1530707711204098</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>773.15</v>
+      </c>
+      <c r="K11">
+        <v>3.2934131736526999</v>
+      </c>
+      <c r="M11">
+        <v>723.15</v>
+      </c>
+      <c r="N11">
+        <v>2.52095808383234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>1373.5025680574099</v>
       </c>
@@ -3406,8 +4047,14 @@
       <c r="E12" s="2">
         <v>1.93508299700286</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>723.71179775280802</v>
+      </c>
+      <c r="N12">
+        <v>2.16160936553859</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>1567.3384808432399</v>
       </c>
@@ -3420,13 +4067,33 @@
       <c r="E13" s="2">
         <v>1.71709522288535</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>773.15</v>
+      </c>
+      <c r="N13">
+        <v>3.6526946107784499</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D14" s="2">
         <v>1577.32637129984</v>
       </c>
       <c r="E14" s="2">
         <v>0.84514412641520598</v>
+      </c>
+      <c r="M14">
+        <v>774.27359550561698</v>
+      </c>
+      <c r="N14">
+        <v>1.67651214425082</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>572.02640449438195</v>
+      </c>
+      <c r="N15">
+        <v>8.39668976653484E-2</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3448,11 +4115,14 @@
       <c r="E36" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="M1:N1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="A35:E35"/>
-    <mergeCell ref="A36:E36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5650,21 +6320,583 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D45C8D-0E1D-4271-9C84-7C91BB3EB92B}">
-  <dimension ref="A52"/>
+  <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8" style="8"/>
+    <col min="1" max="2" width="13.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" style="2" customWidth="1"/>
+    <col min="4" max="5" width="13.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" style="2" customWidth="1"/>
+    <col min="7" max="8" width="13.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="4.28515625" style="2" customWidth="1"/>
+    <col min="10" max="11" width="13.28515625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="4.28515625" style="2" customWidth="1"/>
+    <col min="13" max="14" width="13.28515625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="4.28515625" style="2" customWidth="1"/>
+    <col min="16" max="17" width="13.28515625" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="8" style="2"/>
   </cols>
   <sheetData>
-    <row r="52" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="D1" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="12"/>
+      <c r="G1" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="12"/>
+      <c r="J1" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="12"/>
+      <c r="M1" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="N1" s="12"/>
+      <c r="P1" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q1" s="12"/>
+    </row>
+    <row r="3" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>34.3480892776941</v>
+      </c>
+      <c r="B4">
+        <v>175.56626506024</v>
+      </c>
+      <c r="D4">
+        <v>32.567221885922898</v>
+      </c>
+      <c r="E4">
+        <v>167.662650602409</v>
+      </c>
+      <c r="G4">
+        <v>32.161059147448803</v>
+      </c>
+      <c r="H4">
+        <v>147.61445783132501</v>
+      </c>
+      <c r="J4">
+        <v>26.552889027747899</v>
+      </c>
+      <c r="K4">
+        <v>110.795180722891</v>
+      </c>
+      <c r="M4">
+        <v>31.458085177012698</v>
+      </c>
+      <c r="N4">
+        <v>112.915662650602</v>
+      </c>
+      <c r="P4">
+        <v>21.350881646521199</v>
+      </c>
+      <c r="Q4">
+        <v>174.02409638554201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>105.68042022221699</v>
+      </c>
+      <c r="B5">
+        <v>176.53012048192701</v>
+      </c>
+      <c r="D5">
+        <v>98.9006268184569</v>
+      </c>
+      <c r="E5">
+        <v>161.87951807228899</v>
+      </c>
+      <c r="G5">
+        <v>96.881529358926699</v>
+      </c>
+      <c r="H5">
+        <v>142.21686746987899</v>
+      </c>
+      <c r="J5">
+        <v>99.474722227646396</v>
+      </c>
+      <c r="K5">
+        <v>110.21686746987901</v>
+      </c>
+      <c r="M5">
+        <v>99.564546679424296</v>
+      </c>
+      <c r="N5">
+        <v>114.650602409638</v>
+      </c>
+      <c r="P5">
+        <v>97.408759836753703</v>
+      </c>
+      <c r="Q5">
+        <v>168.240963855421</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>204.221749233563</v>
+      </c>
+      <c r="B6">
+        <v>160.53012048192701</v>
+      </c>
+      <c r="D6">
+        <v>200.85919040831001</v>
+      </c>
+      <c r="E6">
+        <v>154.55421686746899</v>
+      </c>
+      <c r="G6">
+        <v>201.89412430922999</v>
+      </c>
+      <c r="H6">
+        <v>125.63855421686701</v>
+      </c>
+      <c r="J6">
+        <v>196.66087364042801</v>
+      </c>
+      <c r="K6">
+        <v>107.325301204819</v>
+      </c>
+      <c r="M6">
+        <v>198.40659233367799</v>
+      </c>
+      <c r="N6">
+        <v>113.493975903614</v>
+      </c>
+      <c r="P6">
+        <v>200.765460545585</v>
+      </c>
+      <c r="Q6">
+        <v>149.92771084337301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>302.82165940911102</v>
+      </c>
+      <c r="B7">
+        <v>147.42168674698701</v>
+      </c>
+      <c r="D7">
+        <v>301.138427291011</v>
+      </c>
+      <c r="E7">
+        <v>144.33734939759</v>
+      </c>
+      <c r="G7">
+        <v>302.235847767081</v>
+      </c>
+      <c r="H7">
+        <v>118.506024096385</v>
+      </c>
+      <c r="J7">
+        <v>300.34172345784998</v>
+      </c>
+      <c r="K7">
+        <v>105.012048192771</v>
+      </c>
+      <c r="M7">
+        <v>303.688660639315</v>
+      </c>
+      <c r="N7">
+        <v>110.21686746987901</v>
+      </c>
+      <c r="P7">
+        <v>297.80711175333403</v>
+      </c>
+      <c r="Q7">
+        <v>139.903614457831</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>401.56606978969302</v>
+      </c>
+      <c r="B8">
+        <v>141.44578313253001</v>
+      </c>
+      <c r="D8">
+        <v>399.87112143875299</v>
+      </c>
+      <c r="E8">
+        <v>137.78313253012001</v>
+      </c>
+      <c r="G8">
+        <v>402.72207142996598</v>
+      </c>
+      <c r="H8">
+        <v>118.506024096385</v>
+      </c>
+      <c r="J8">
+        <v>402.48384136220699</v>
+      </c>
+      <c r="K8">
+        <v>106.746987951807</v>
+      </c>
+      <c r="M8">
+        <v>400.945109449141</v>
+      </c>
+      <c r="N8">
+        <v>110.795180722891</v>
+      </c>
+      <c r="P8">
+        <v>399.78910780886901</v>
+      </c>
+      <c r="Q8">
+        <v>133.734939759036</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>501.98199605553401</v>
+      </c>
+      <c r="B9">
+        <v>137.975903614457</v>
+      </c>
+      <c r="D9">
+        <v>503.56368748901502</v>
+      </c>
+      <c r="E9">
+        <v>136.04819277108399</v>
+      </c>
+      <c r="G9">
+        <v>503.20048427095702</v>
+      </c>
+      <c r="H9">
+        <v>118.12048192771</v>
+      </c>
+      <c r="J9">
+        <v>502.98178125793203</v>
+      </c>
+      <c r="K9">
+        <v>107.325301204819</v>
+      </c>
+      <c r="M9">
+        <v>504.68844584171302</v>
+      </c>
+      <c r="N9">
+        <v>111.56626506024</v>
+      </c>
+      <c r="P9">
+        <v>501.78282009724398</v>
+      </c>
+      <c r="Q9">
+        <v>128.14457831325299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>602.36277362285398</v>
+      </c>
+      <c r="B10">
+        <v>132.77108433734901</v>
+      </c>
+      <c r="D10">
+        <v>602.34324656811998</v>
+      </c>
+      <c r="E10">
+        <v>131.80722891566199</v>
+      </c>
+      <c r="G10">
+        <v>603.64765382437304</v>
+      </c>
+      <c r="H10">
+        <v>116.192771084337</v>
+      </c>
+      <c r="J10">
+        <v>600.21479760207706</v>
+      </c>
+      <c r="K10">
+        <v>106.746987951807</v>
+      </c>
+      <c r="M10">
+        <v>603.550018550701</v>
+      </c>
+      <c r="N10">
+        <v>111.373493975903</v>
+      </c>
+      <c r="P10">
+        <v>600.56237917634803</v>
+      </c>
+      <c r="Q10">
+        <v>123.903614457831</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>704.35648591122902</v>
+      </c>
+      <c r="B11">
+        <v>127.18072289156601</v>
+      </c>
+      <c r="D11">
+        <v>701.138427291011</v>
+      </c>
+      <c r="E11">
+        <v>128.33734939759</v>
+      </c>
+      <c r="G11">
+        <v>700.89238640135795</v>
+      </c>
+      <c r="H11">
+        <v>116.192771084337</v>
+      </c>
+      <c r="J11">
+        <v>700.69321044306798</v>
+      </c>
+      <c r="K11">
+        <v>106.361445783132</v>
+      </c>
+      <c r="M11">
+        <v>700.78303489484597</v>
+      </c>
+      <c r="N11">
+        <v>110.795180722891</v>
+      </c>
+      <c r="P11">
+        <v>699.36927613208002</v>
+      </c>
+      <c r="Q11">
+        <v>121.012048192771</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>801.48405615980903</v>
+      </c>
+      <c r="B12">
+        <v>121.397590361445</v>
+      </c>
+      <c r="D12">
+        <v>799.92189178106196</v>
+      </c>
+      <c r="E12">
+        <v>124.289156626506</v>
+      </c>
+      <c r="G12">
+        <v>802.995450196246</v>
+      </c>
+      <c r="H12">
+        <v>116</v>
+      </c>
+      <c r="J12">
+        <v>801.19115033879405</v>
+      </c>
+      <c r="K12">
+        <v>106.939759036144</v>
+      </c>
+      <c r="M12">
+        <v>798.027767471831</v>
+      </c>
+      <c r="N12">
+        <v>110.795180722891</v>
+      </c>
+      <c r="P12">
+        <v>803.03840971666204</v>
+      </c>
+      <c r="Q12">
+        <v>118.12048192771</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>901.91560406943802</v>
+      </c>
+      <c r="B13">
+        <v>118.698795180722</v>
+      </c>
+      <c r="D13">
+        <v>901.96246900079996</v>
+      </c>
+      <c r="E13">
+        <v>121.012048192771</v>
+      </c>
+      <c r="G13">
+        <v>901.860928316181</v>
+      </c>
+      <c r="H13">
+        <v>116</v>
+      </c>
+      <c r="J13">
+        <v>901.66565776883795</v>
+      </c>
+      <c r="K13">
+        <v>106.361445783132</v>
+      </c>
+      <c r="M13">
+        <v>903.32545742125706</v>
+      </c>
+      <c r="N13">
+        <v>108.289156626506</v>
+      </c>
+      <c r="P13">
+        <v>901.896077014703</v>
+      </c>
+      <c r="Q13">
+        <v>117.734939759036</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1002.43697643084</v>
+      </c>
+      <c r="B14">
+        <v>120.43373493975901</v>
+      </c>
+      <c r="D14">
+        <v>1002.49946300599</v>
+      </c>
+      <c r="E14">
+        <v>123.518072289156</v>
+      </c>
+      <c r="G14">
+        <v>1002.3510573900101</v>
+      </c>
+      <c r="H14">
+        <v>116.192771084337</v>
+      </c>
+      <c r="J14">
+        <v>1003.85073519361</v>
+      </c>
+      <c r="K14">
+        <v>110.21686746987901</v>
+      </c>
+      <c r="M14">
+        <v>1000.64829821717</v>
+      </c>
+      <c r="N14">
+        <v>112.14457831325301</v>
+      </c>
+      <c r="P14">
+        <v>1003.9913299876901</v>
+      </c>
+      <c r="Q14">
+        <v>117.156626506024</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1081.84569721348</v>
+      </c>
+      <c r="B15">
+        <v>120.048192771084</v>
+      </c>
+      <c r="D15">
+        <v>1080.25619495811</v>
+      </c>
+      <c r="E15">
+        <v>121.590361445783</v>
+      </c>
+      <c r="G15">
+        <v>1081.7793052273901</v>
+      </c>
+      <c r="H15">
+        <v>116.771084337349</v>
+      </c>
+      <c r="J15">
+        <v>1080.10778934213</v>
+      </c>
+      <c r="K15">
+        <v>114.265060240963</v>
+      </c>
+      <c r="M15">
+        <v>1080.0726406436099</v>
+      </c>
+      <c r="N15">
+        <v>112.530120481927</v>
+      </c>
+      <c r="P15">
+        <v>1083.38442912655</v>
+      </c>
+      <c r="Q15">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
+      <c r="N38" s="12"/>
+      <c r="O38" s="12"/>
+      <c r="P38" s="12"/>
+      <c r="Q38" s="12"/>
+    </row>
+    <row r="52" s="2" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A38:Q38"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="P1:Q1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add Fit functions for Tungsten Fatigue
</commit_message>
<xml_diff>
--- a/Jupyter/Tungsten/Tungsten.xlsx
+++ b/Jupyter/Tungsten/Tungsten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuqih\Documents\GitHub\DatabaseCodes\Jupyter\Tungsten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63ED68A-2479-4F2A-B586-E63E77906AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8139DED-D649-43B3-9C91-97C5DF23E991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="852" firstSheet="5" activeTab="16" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="852" firstSheet="16" activeTab="17" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
   </bookViews>
   <sheets>
     <sheet name="W_density" sheetId="15" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="133">
   <si>
     <t>W-Fujitsuka</t>
   </si>
@@ -342,31 +342,7 @@
     <t>Stress (Mpa)</t>
   </si>
   <si>
-    <t>W RLU</t>
-  </si>
-  <si>
-    <t>W RLP</t>
-  </si>
-  <si>
-    <t>W FU</t>
-  </si>
-  <si>
-    <t>W FP</t>
-  </si>
-  <si>
     <t>Fig 8. Habainy, Jemila, et al. "Fatigue behavior of rolled and forged tungsten at 25, 280 and 480 C." Journal of Nuclear Materials 465 (2015): 438-447.</t>
-  </si>
-  <si>
-    <t>W 280C RLP</t>
-  </si>
-  <si>
-    <t>W 280 FU</t>
-  </si>
-  <si>
-    <t>W 280 FP</t>
-  </si>
-  <si>
-    <t>W 480 FP</t>
   </si>
   <si>
     <t>Fig 9. Habainy, Jemila, et al. "Fatigue behavior of rolled and forged tungsten at 25, 280 and 480 C." Journal of Nuclear Materials 465 (2015): 438-447.</t>
@@ -570,22 +546,43 @@
     <t>sigma</t>
   </si>
   <si>
-    <t>W epsdot Conway</t>
-  </si>
-  <si>
-    <t>W epsdot Klopp1</t>
-  </si>
-  <si>
-    <t>W epsdot Klopp2</t>
-  </si>
-  <si>
-    <t>W  epsdot Green</t>
-  </si>
-  <si>
-    <t>W epsdot Harris</t>
-  </si>
-  <si>
     <t>W epsdot King</t>
+  </si>
+  <si>
+    <t>W epsdot Flagella</t>
+  </si>
+  <si>
+    <t>W epsdot Klopp</t>
+  </si>
+  <si>
+    <t>W epsdot Green</t>
+  </si>
+  <si>
+    <t>W epsdot Gilbert</t>
+  </si>
+  <si>
+    <t>W RLU_</t>
+  </si>
+  <si>
+    <t>W RLP_</t>
+  </si>
+  <si>
+    <t>W FU_</t>
+  </si>
+  <si>
+    <t>W FP_</t>
+  </si>
+  <si>
+    <t>W 280C RLP_</t>
+  </si>
+  <si>
+    <t>W 280 FU_</t>
+  </si>
+  <si>
+    <t>W 280 FP_</t>
+  </si>
+  <si>
+    <t>W 480 FP_</t>
   </si>
 </sst>
 </file>
@@ -722,6 +719,12 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -736,12 +739,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1323,16 +1320,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>48</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>21728</xdr:rowOff>
+      <xdr:rowOff>88403</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>54</xdr:col>
-      <xdr:colOff>524622</xdr:colOff>
+      <xdr:col>50</xdr:col>
+      <xdr:colOff>572247</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>48494</xdr:rowOff>
+      <xdr:rowOff>115169</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1355,7 +1352,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="36109275" y="3869828"/>
+          <a:off x="33718500" y="3936503"/>
           <a:ext cx="4115547" cy="4789266"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2416,35 +2413,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="16"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="14"/>
+      <c r="E1" s="16"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="14"/>
+      <c r="H1" s="16"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="14"/>
+      <c r="K1" s="16"/>
       <c r="L1" s="2"/>
-      <c r="M1" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="N1" s="14"/>
+      <c r="M1" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" s="16"/>
       <c r="O1" s="2"/>
-      <c r="P1" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q1" s="14"/>
+      <c r="P1" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" s="16"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -3464,46 +3461,46 @@
       <c r="Q37" s="2"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A49" s="14" t="s">
+      <c r="A49" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-      <c r="K49" s="14"/>
-      <c r="L49" s="14"/>
-      <c r="M49" s="14"/>
-      <c r="N49" s="14"/>
-      <c r="O49" s="14"/>
-      <c r="P49" s="14"/>
-      <c r="Q49" s="14"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16"/>
+      <c r="I49" s="16"/>
+      <c r="J49" s="16"/>
+      <c r="K49" s="16"/>
+      <c r="L49" s="16"/>
+      <c r="M49" s="16"/>
+      <c r="N49" s="16"/>
+      <c r="O49" s="16"/>
+      <c r="P49" s="16"/>
+      <c r="Q49" s="16"/>
     </row>
     <row r="52" spans="1:17" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="14" t="s">
+      <c r="A52" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
-      <c r="M52" s="14"/>
-      <c r="N52" s="14"/>
-      <c r="O52" s="14"/>
-      <c r="P52" s="14"/>
-      <c r="Q52" s="14"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="16"/>
+      <c r="J52" s="16"/>
+      <c r="K52" s="16"/>
+      <c r="L52" s="16"/>
+      <c r="M52" s="16"/>
+      <c r="N52" s="16"/>
+      <c r="O52" s="16"/>
+      <c r="P52" s="16"/>
+      <c r="Q52" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3581,14 +3578,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="D1" s="14" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="14"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -3762,13 +3759,13 @@
       <c r="F34" s="1"/>
     </row>
     <row r="37" spans="1:6" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3804,58 +3801,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="16"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="14"/>
-      <c r="G1" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="H1" s="16"/>
-      <c r="J1" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="K1" s="16"/>
-      <c r="M1" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="N1" s="16"/>
+      <c r="D1" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="16"/>
+      <c r="G1" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="18"/>
+      <c r="J1" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="18"/>
+      <c r="M1" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="N1" s="18"/>
     </row>
     <row r="3" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -4251,22 +4248,22 @@
       </c>
     </row>
     <row r="32" spans="1:14" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
+      <c r="A32" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
     </row>
     <row r="33" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
+      <c r="A33" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -4306,59 +4303,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="D1" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="E1" s="14"/>
-      <c r="G1" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="H1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="D1" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="16"/>
+      <c r="G1" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="18"/>
       <c r="I1"/>
-      <c r="J1" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="K1" s="16"/>
+      <c r="J1" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="18"/>
       <c r="L1"/>
-      <c r="M1" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="N1" s="16"/>
+      <c r="M1" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="N1" s="18"/>
     </row>
     <row r="3" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -4668,22 +4665,22 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
+      <c r="A35" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
     </row>
     <row r="36" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
+      <c r="A36" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -4715,15 +4712,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="B1" s="14"/>
+      <c r="A1" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="16"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="E1" s="14"/>
+      <c r="D1" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -4737,14 +4734,14 @@
         <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -4864,13 +4861,13 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
+      <c r="A34" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4903,14 +4900,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="D1" s="14" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="14"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -5027,13 +5024,13 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5095,63 +5092,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="D1" s="14" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="16"/>
+      <c r="G1" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="19"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="K1" s="19"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="N1" s="19"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="T1" s="19"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="W1" s="19"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC1" s="19"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="17" t="s">
+      <c r="AF1" s="19"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="N1" s="17"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="T1" s="17"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="W1" s="17"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="Z1" s="17"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="AC1" s="17"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="AF1" s="17"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="AI1" s="17"/>
+      <c r="AI1" s="19"/>
     </row>
     <row r="3" spans="1:35" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -5812,21 +5809,16 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="J1:K1"/>
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AH1:AI1"/>
@@ -5835,6 +5827,11 @@
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5843,10 +5840,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE9D7C7B-E4E9-42EA-9DB0-66C5C7498970}">
-  <dimension ref="A1:BG54"/>
+  <dimension ref="A1:BD54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI23" workbookViewId="0">
-      <selection activeCell="BD40" sqref="BD40"/>
+    <sheetView topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="BD20" sqref="BD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5874,89 +5871,85 @@
     <col min="42" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="D1" s="14" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="G1" s="14" t="s">
+      <c r="E1" s="16"/>
+      <c r="G1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="J1" s="14" t="s">
+      <c r="H1" s="16"/>
+      <c r="J1" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="M1" s="14" t="s">
+      <c r="K1" s="16"/>
+      <c r="M1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="14"/>
-      <c r="P1" s="14" t="s">
+      <c r="N1" s="16"/>
+      <c r="P1" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" s="14"/>
-      <c r="S1" s="14" t="s">
+      <c r="Q1" s="16"/>
+      <c r="S1" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="14"/>
-      <c r="V1" s="14" t="s">
+      <c r="T1" s="16"/>
+      <c r="V1" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="W1" s="14"/>
-      <c r="Y1" s="14" t="s">
+      <c r="W1" s="16"/>
+      <c r="Y1" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="Z1" s="14"/>
-      <c r="AB1" s="14" t="s">
+      <c r="Z1" s="16"/>
+      <c r="AB1" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="AC1" s="14"/>
-      <c r="AE1" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF1" s="14"/>
-      <c r="AH1" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="AI1" s="14"/>
-      <c r="AK1" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="AL1" s="14"/>
-      <c r="AN1" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="AO1" s="14"/>
-      <c r="AQ1" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="AR1" s="14"/>
-      <c r="AT1" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="AU1" s="14"/>
-      <c r="AW1" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="AX1" s="14"/>
-      <c r="AZ1" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="BA1" s="14"/>
-      <c r="BC1" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="BD1" s="14"/>
-      <c r="BF1" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="BG1" s="14"/>
-    </row>
-    <row r="3" spans="1:59" ht="33" x14ac:dyDescent="0.25">
+      <c r="AC1" s="16"/>
+      <c r="AE1" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="AF1" s="16"/>
+      <c r="AH1" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI1" s="16"/>
+      <c r="AK1" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="AL1" s="16"/>
+      <c r="AN1" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO1" s="16"/>
+      <c r="AQ1" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="AR1" s="16"/>
+      <c r="AT1" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="AU1" s="16"/>
+      <c r="AW1" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="AX1" s="16"/>
+      <c r="AZ1" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="BA1" s="16"/>
+      <c r="BC1" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD1" s="16"/>
+    </row>
+    <row r="3" spans="1:56" ht="33" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -6018,70 +6011,64 @@
         <v>32</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="AH3" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="AI3" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="AK3" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="AL3" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="AN3" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="AO3" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="AQ3" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="AR3" s="2" t="s">
-        <v>126</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="AS3" s="13"/>
       <c r="AT3" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="AU3" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="AV3" s="18"/>
+        <v>118</v>
+      </c>
+      <c r="AV3" s="13"/>
       <c r="AW3" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="AX3" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="AY3" s="18"/>
+        <v>118</v>
+      </c>
+      <c r="AY3" s="13"/>
       <c r="AZ3" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="BA3" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="BB3" s="18"/>
+        <v>118</v>
+      </c>
       <c r="BC3" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="BD3" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="BF3" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="BG3" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>147.320952997912</v>
       </c>
@@ -6100,46 +6087,46 @@
       <c r="H4" s="2">
         <v>4.7474747474747403</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="14">
         <v>134.95213416828599</v>
       </c>
-      <c r="K4" s="19">
+      <c r="K4" s="14">
         <v>7.6565656565656504</v>
       </c>
-      <c r="M4" s="19">
+      <c r="M4" s="14">
         <v>137.09637947167599</v>
       </c>
-      <c r="N4" s="19">
+      <c r="N4" s="14">
         <v>7.8383838383838302</v>
       </c>
-      <c r="P4" s="19">
+      <c r="P4" s="14">
         <v>152.731331430165</v>
       </c>
-      <c r="Q4" s="19">
+      <c r="Q4" s="14">
         <v>2.54899225138981</v>
       </c>
-      <c r="S4" s="19">
+      <c r="S4" s="14">
         <v>149.647985575994</v>
       </c>
-      <c r="T4" s="19">
+      <c r="T4" s="14">
         <v>2.62443924531541</v>
       </c>
-      <c r="V4" s="19">
+      <c r="V4" s="14">
         <v>146.285603897915</v>
       </c>
-      <c r="W4" s="19">
+      <c r="W4" s="14">
         <v>2.6614651527184501</v>
       </c>
-      <c r="Y4" s="19">
+      <c r="Y4" s="14">
         <v>9.1502285947326492</v>
       </c>
-      <c r="Z4" s="19">
+      <c r="Z4" s="14">
         <v>18.394363476357</v>
       </c>
-      <c r="AB4" s="19">
+      <c r="AB4" s="14">
         <v>31.712421387022601</v>
       </c>
-      <c r="AC4" s="19">
+      <c r="AC4" s="14">
         <v>12.9240807916031</v>
       </c>
       <c r="AE4" s="2">
@@ -6166,48 +6153,41 @@
       <c r="AO4" s="2">
         <v>22.2008676815414</v>
       </c>
-      <c r="AQ4" s="8">
-        <v>-2.2554436652390901</v>
-      </c>
-      <c r="AR4" s="8">
-        <v>-10.9371917865206</v>
-      </c>
-      <c r="AS4" s="19"/>
-      <c r="AT4" s="8">
-        <v>-1.35300472555888</v>
-      </c>
-      <c r="AU4" s="8">
-        <v>-7.8791312333077403</v>
-      </c>
-      <c r="AV4" s="19"/>
-      <c r="AW4" s="8">
-        <v>-1.6524477139829701</v>
-      </c>
-      <c r="AX4" s="8">
-        <v>-7.1899149534652702</v>
-      </c>
-      <c r="AY4" s="19"/>
-      <c r="AZ4" s="8">
-        <v>-1.3823822718819201</v>
-      </c>
-      <c r="BA4" s="8">
-        <v>-9.4134016125433302</v>
-      </c>
-      <c r="BB4" s="19"/>
-      <c r="BC4" s="8">
-        <v>-0.35493693170636198</v>
-      </c>
-      <c r="BD4" s="8">
-        <v>-2.8531478579397</v>
-      </c>
-      <c r="BF4" s="8">
-        <v>-1.2494879892413</v>
-      </c>
-      <c r="BG4" s="8">
-        <v>-7.0849463857534998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="AQ4">
+        <v>-3.7765826409570802</v>
+      </c>
+      <c r="AR4">
+        <v>9.2668898730954794</v>
+      </c>
+      <c r="AS4" s="14"/>
+      <c r="AT4">
+        <v>-3.3964105720707298</v>
+      </c>
+      <c r="AU4">
+        <v>12.8600035479431</v>
+      </c>
+      <c r="AV4" s="14"/>
+      <c r="AW4">
+        <v>-3.9238832848383098</v>
+      </c>
+      <c r="AX4">
+        <v>6.7073583737445999</v>
+      </c>
+      <c r="AY4" s="14"/>
+      <c r="AZ4">
+        <v>-3.5932640438480399</v>
+      </c>
+      <c r="BA4">
+        <v>10.150253995158399</v>
+      </c>
+      <c r="BC4">
+        <v>-3.3803729572324301</v>
+      </c>
+      <c r="BD4">
+        <v>12.243874398479401</v>
+      </c>
+    </row>
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>155.486935866983</v>
       </c>
@@ -6226,46 +6206,46 @@
       <c r="H5" s="2">
         <v>3.9393939393939399</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="14">
         <v>163.72921615201801</v>
       </c>
-      <c r="K5" s="19">
+      <c r="K5" s="14">
         <v>5.3333333333333304</v>
       </c>
-      <c r="M5" s="19">
+      <c r="M5" s="14">
         <v>164.42453033901899</v>
       </c>
-      <c r="N5" s="19">
+      <c r="N5" s="14">
         <v>4.8484848484848504</v>
       </c>
-      <c r="P5" s="19">
+      <c r="P5" s="14">
         <v>165.35126317371001</v>
       </c>
-      <c r="Q5" s="19">
+      <c r="Q5" s="14">
         <v>2.0174290068471001</v>
       </c>
-      <c r="S5" s="19">
+      <c r="S5" s="14">
         <v>161.70984567172499</v>
       </c>
-      <c r="T5" s="19">
+      <c r="T5" s="14">
         <v>2.0160338277275698</v>
       </c>
-      <c r="V5" s="19">
+      <c r="V5" s="14">
         <v>158.06735495503199</v>
       </c>
-      <c r="W5" s="19">
+      <c r="W5" s="14">
         <v>2.0529524136598698</v>
       </c>
-      <c r="Y5" s="19">
+      <c r="Y5" s="14">
         <v>30.5662280795895</v>
       </c>
-      <c r="Z5" s="19">
+      <c r="Z5" s="14">
         <v>13.843181866964301</v>
       </c>
-      <c r="AB5" s="19">
+      <c r="AB5" s="14">
         <v>40.766060658095199</v>
       </c>
-      <c r="AC5" s="19">
+      <c r="AC5" s="14">
         <v>9.7091588143123904</v>
       </c>
       <c r="AE5" s="2">
@@ -6292,48 +6272,41 @@
       <c r="AO5" s="2">
         <v>21.678808143617399</v>
       </c>
-      <c r="AQ5" s="8">
-        <v>-2.1174796616120899</v>
-      </c>
-      <c r="AR5" s="8">
-        <v>-10.048204341394401</v>
-      </c>
-      <c r="AS5" s="19"/>
-      <c r="AT5" s="8">
-        <v>-1.3152584836228001</v>
-      </c>
-      <c r="AU5" s="8">
-        <v>-7.4305635630923303</v>
-      </c>
-      <c r="AV5" s="19"/>
-      <c r="AW5" s="8">
-        <v>-1.31874438489165</v>
-      </c>
-      <c r="AX5" s="8">
-        <v>-7.4655034173284696</v>
-      </c>
-      <c r="AY5" s="19"/>
-      <c r="AZ5" s="8">
-        <v>-1.33773447562448</v>
-      </c>
-      <c r="BA5" s="8">
-        <v>-9.1816272719488392</v>
-      </c>
-      <c r="BB5" s="19"/>
-      <c r="BC5" s="8">
-        <v>-0.22019493136214799</v>
-      </c>
-      <c r="BD5" s="8">
-        <v>-2.43287877208114</v>
-      </c>
-      <c r="BF5" s="8">
-        <v>-1.16836011573823</v>
-      </c>
-      <c r="BG5" s="8">
-        <v>-6.5134696477107399</v>
-      </c>
-    </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="AQ5">
+        <v>-3.8529395171648702</v>
+      </c>
+      <c r="AR5">
+        <v>8.8809843515512892</v>
+      </c>
+      <c r="AS5" s="14"/>
+      <c r="AT5">
+        <v>-3.63497771531974</v>
+      </c>
+      <c r="AU5">
+        <v>10.4475619674788</v>
+      </c>
+      <c r="AV5" s="14"/>
+      <c r="AW5">
+        <v>-3.9260190110653701</v>
+      </c>
+      <c r="AX5">
+        <v>6.5660110953586699</v>
+      </c>
+      <c r="AY5" s="14"/>
+      <c r="AZ5">
+        <v>-3.5467642546910101</v>
+      </c>
+      <c r="BA5">
+        <v>10.2647919453574</v>
+      </c>
+      <c r="BC5">
+        <v>-3.4746247666150198</v>
+      </c>
+      <c r="BD5">
+        <v>11.661777128348</v>
+      </c>
+    </row>
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>165.78420787446899</v>
       </c>
@@ -6352,46 +6325,46 @@
       <c r="H6" s="2">
         <v>2.9696969696969702</v>
       </c>
-      <c r="J6" s="19">
+      <c r="J6" s="14">
         <v>192.87338947671401</v>
       </c>
-      <c r="K6" s="19">
+      <c r="K6" s="14">
         <v>3.31313131313131</v>
       </c>
-      <c r="M6" s="19">
+      <c r="M6" s="14">
         <v>193.21816742244201</v>
       </c>
-      <c r="N6" s="19">
+      <c r="N6" s="14">
         <v>2.9898989898989901</v>
       </c>
-      <c r="P6" s="19">
+      <c r="P6" s="14">
         <v>175.16688488699</v>
       </c>
-      <c r="Q6" s="19">
+      <c r="Q6" s="14">
         <v>1.59973384275258</v>
       </c>
-      <c r="S6" s="19">
+      <c r="S6" s="14">
         <v>171.52332095559001</v>
       </c>
-      <c r="T6" s="19">
+      <c r="T6" s="14">
         <v>1.67496619373671</v>
       </c>
-      <c r="V6" s="19">
+      <c r="V6" s="14">
         <v>167.60286762969699</v>
       </c>
-      <c r="W6" s="19">
+      <c r="W6" s="14">
         <v>1.63514992809461</v>
       </c>
-      <c r="Y6" s="19">
+      <c r="Y6" s="14">
         <v>40.403314087016199</v>
       </c>
-      <c r="Z6" s="19">
+      <c r="Z6" s="14">
         <v>12.659211401833</v>
       </c>
-      <c r="AB6" s="19">
+      <c r="AB6" s="14">
         <v>53.690785378522797</v>
       </c>
-      <c r="AC6" s="19">
+      <c r="AC6" s="14">
         <v>8.2964862950481795</v>
       </c>
       <c r="AE6" s="2">
@@ -6418,48 +6391,41 @@
       <c r="AO6" s="2">
         <v>21.014813919694699</v>
       </c>
-      <c r="AQ6" s="8">
-        <v>-2.0869012179764699</v>
-      </c>
-      <c r="AR6" s="8">
-        <v>-10.1259196166554</v>
-      </c>
-      <c r="AS6" s="19"/>
-      <c r="AT6" s="8">
-        <v>-1.2636805347056701</v>
-      </c>
-      <c r="AU6" s="8">
-        <v>-7.22107793459148</v>
-      </c>
-      <c r="AV6" s="19"/>
-      <c r="AW6" s="8">
-        <v>-1.1989059941223901</v>
-      </c>
-      <c r="AX6" s="8">
-        <v>-6.7000227793437803</v>
-      </c>
-      <c r="AY6" s="19"/>
-      <c r="AZ6" s="8">
-        <v>-1.3010124104343801</v>
-      </c>
-      <c r="BA6" s="8">
-        <v>-9.1510217913009697</v>
-      </c>
-      <c r="BB6" s="19"/>
-      <c r="BC6" s="8">
-        <v>-0.20787161374482899</v>
-      </c>
-      <c r="BD6" s="8">
-        <v>-2.3966555264849001</v>
-      </c>
-      <c r="BF6" s="8">
-        <v>-1.10928646592375</v>
-      </c>
-      <c r="BG6" s="8">
-        <v>-6.0738399078112604</v>
-      </c>
-    </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="AQ6">
+        <v>-3.91263623793302</v>
+      </c>
+      <c r="AR6">
+        <v>8.5648540620690401</v>
+      </c>
+      <c r="AS6" s="14"/>
+      <c r="AT6">
+        <v>-3.6911524553688699</v>
+      </c>
+      <c r="AU6">
+        <v>10.251896407107701</v>
+      </c>
+      <c r="AV6" s="14"/>
+      <c r="AW6">
+        <v>-4.0197538866754297</v>
+      </c>
+      <c r="AX6">
+        <v>6.5187845955472099</v>
+      </c>
+      <c r="AY6" s="14"/>
+      <c r="AZ6">
+        <v>-3.5060727342096398</v>
+      </c>
+      <c r="BA6">
+        <v>10.1367868838782</v>
+      </c>
+      <c r="BC6">
+        <v>-3.4973957770445701</v>
+      </c>
+      <c r="BD6">
+        <v>11.349406061654999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>175.01907435399099</v>
       </c>
@@ -6478,28 +6444,28 @@
       <c r="H7" s="2">
         <v>2.1414141414141401</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="14">
         <v>221.69797739869</v>
       </c>
-      <c r="K7" s="19">
+      <c r="K7" s="14">
         <v>2.32323232323232</v>
       </c>
-      <c r="M7" s="19">
+      <c r="M7" s="14">
         <v>220.24976606924301</v>
       </c>
-      <c r="N7" s="19">
+      <c r="N7" s="14">
         <v>1.67676767676767</v>
       </c>
-      <c r="Y7" s="19">
+      <c r="Y7" s="14">
         <v>53.056515486488202</v>
       </c>
-      <c r="Z7" s="19">
+      <c r="Z7" s="14">
         <v>10.939921440683399</v>
       </c>
-      <c r="AB7" s="19">
+      <c r="AB7" s="14">
         <v>63.534310674193399</v>
       </c>
-      <c r="AC7" s="19">
+      <c r="AC7" s="14">
         <v>6.8826332396059096</v>
       </c>
       <c r="AE7" s="2">
@@ -6526,58 +6492,51 @@
       <c r="AO7" s="2">
         <v>19.0969076086262</v>
       </c>
-      <c r="AQ7" s="8">
-        <v>-2.07358907501759</v>
-      </c>
-      <c r="AR7" s="8">
-        <v>-9.4486290890066194</v>
-      </c>
-      <c r="AS7" s="19"/>
-      <c r="AT7" s="8">
-        <v>-1.2505589306156299</v>
-      </c>
-      <c r="AU7" s="8">
-        <v>-7.0908695434101201</v>
-      </c>
-      <c r="AV7" s="19"/>
-      <c r="AW7" s="8">
-        <v>-1.14298572353675</v>
-      </c>
-      <c r="AX7" s="8">
-        <v>-6.3575932539395597</v>
-      </c>
-      <c r="AY7" s="19"/>
-      <c r="AZ7" s="8">
-        <v>-1.2703663255004101</v>
-      </c>
-      <c r="BA7" s="8">
-        <v>-8.9732934473508106</v>
-      </c>
-      <c r="BB7" s="19"/>
-      <c r="BC7" s="8">
-        <v>-0.19384940472586101</v>
-      </c>
-      <c r="BD7" s="8">
-        <v>-2.1641992028263499</v>
-      </c>
-      <c r="BF7" s="8">
-        <v>-0.95844682889029498</v>
-      </c>
-      <c r="BG7" s="8">
-        <v>-5.1131451131144896</v>
-      </c>
-    </row>
-    <row r="8" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="Y8" s="19">
+      <c r="AQ7">
+        <v>-4.0293078884499298</v>
+      </c>
+      <c r="AR7">
+        <v>8.1160877752113301</v>
+      </c>
+      <c r="AS7" s="14"/>
+      <c r="AT7">
+        <v>-3.8944802498122</v>
+      </c>
+      <c r="AU7">
+        <v>9.0623375084649602</v>
+      </c>
+      <c r="AV7" s="14"/>
+      <c r="AW7">
+        <v>-3.9992690944801201</v>
+      </c>
+      <c r="AX7">
+        <v>6.3458890952904703</v>
+      </c>
+      <c r="AY7" s="14"/>
+      <c r="AZ7">
+        <v>-3.5541558110701201</v>
+      </c>
+      <c r="BA7">
+        <v>10.0645403884012</v>
+      </c>
+      <c r="BC7">
+        <v>-3.6664067397745699</v>
+      </c>
+      <c r="BD7">
+        <v>10.3430333084846</v>
+      </c>
+    </row>
+    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="Y8" s="14">
         <v>63.716757174440303</v>
       </c>
-      <c r="Z8" s="19">
+      <c r="Z8" s="14">
         <v>10.369293180793701</v>
       </c>
-      <c r="AB8" s="19">
+      <c r="AB8" s="14">
         <v>74.4821739037111</v>
       </c>
-      <c r="AC8" s="19">
+      <c r="AC8" s="14">
         <v>6.0439159458241196</v>
       </c>
       <c r="AE8" s="2">
@@ -6598,58 +6557,51 @@
       <c r="AL8" s="2">
         <v>37.7920429024566</v>
       </c>
-      <c r="AQ8" s="8">
-        <v>-2.0211922547019099</v>
-      </c>
-      <c r="AR8" s="8">
-        <v>-9.6620393808161307</v>
-      </c>
-      <c r="AS8" s="19"/>
-      <c r="AT8" s="8">
-        <v>-1.2031139282424601</v>
-      </c>
-      <c r="AU8" s="8">
-        <v>-7.0334018555069298</v>
-      </c>
-      <c r="AV8" s="19"/>
-      <c r="AW8" s="8">
-        <v>-1.0733834121391099</v>
-      </c>
-      <c r="AX8" s="8">
-        <v>-5.9749466425215303</v>
-      </c>
-      <c r="AY8" s="19"/>
-      <c r="AZ8" s="8">
-        <v>-1.2511108707143299</v>
-      </c>
-      <c r="BA8" s="8">
-        <v>-8.8883374379128597</v>
-      </c>
-      <c r="BB8" s="19"/>
-      <c r="BC8" s="8">
-        <v>-0.18478829753065901</v>
-      </c>
-      <c r="BD8" s="8">
-        <v>-2.0552593804344799</v>
-      </c>
-      <c r="BF8" s="8">
-        <v>-0.88369962433407001</v>
-      </c>
-      <c r="BG8" s="8">
-        <v>-4.5038750763441504</v>
-      </c>
-    </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="Y9" s="19">
+      <c r="AQ8">
+        <v>-4.0528171403061801</v>
+      </c>
+      <c r="AR8">
+        <v>8.0089787714291205</v>
+      </c>
+      <c r="AS8" s="14"/>
+      <c r="AT8">
+        <v>-3.8644325456423698</v>
+      </c>
+      <c r="AU8">
+        <v>8.5846514987376104</v>
+      </c>
+      <c r="AV8" s="14"/>
+      <c r="AW8">
+        <v>-4.0835733816637996</v>
+      </c>
+      <c r="AX8">
+        <v>6.1677675023868401</v>
+      </c>
+      <c r="AY8" s="14"/>
+      <c r="AZ8">
+        <v>-3.6160856463410598</v>
+      </c>
+      <c r="BA8">
+        <v>9.4571365422891294</v>
+      </c>
+      <c r="BC8">
+        <v>-3.6381213760076401</v>
+      </c>
+      <c r="BD8">
+        <v>9.9647518955865308</v>
+      </c>
+    </row>
+    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="Y9" s="14">
         <v>74.657107901006597</v>
       </c>
-      <c r="Z9" s="19">
+      <c r="Z9" s="14">
         <v>9.7987722423748096</v>
       </c>
-      <c r="AB9" s="19">
+      <c r="AB9" s="14">
         <v>99.722037390800395</v>
       </c>
-      <c r="AC9" s="19">
+      <c r="AC9" s="14">
         <v>4.9807894567387097</v>
       </c>
       <c r="AE9" s="2">
@@ -6670,58 +6622,51 @@
       <c r="AL9" s="2">
         <v>37.790287586684002</v>
       </c>
-      <c r="AQ9" s="8">
-        <v>-2.0254566530395799</v>
-      </c>
-      <c r="AR9" s="8">
-        <v>-9.2942561769612499</v>
-      </c>
-      <c r="AS9" s="19"/>
-      <c r="AT9" s="8">
-        <v>-1.1540144810949899</v>
-      </c>
-      <c r="AU9" s="8">
-        <v>-6.9107824911362403</v>
-      </c>
-      <c r="AV9" s="19"/>
-      <c r="AW9" s="8">
-        <v>-1.02545217161506</v>
-      </c>
-      <c r="AX9" s="8">
-        <v>-5.6828766699986204</v>
-      </c>
-      <c r="AY9" s="19"/>
-      <c r="AZ9" s="8">
-        <v>-1.25453516550876</v>
-      </c>
-      <c r="BA9" s="8">
-        <v>-8.6406174557978499</v>
-      </c>
-      <c r="BB9" s="19"/>
-      <c r="BC9" s="8">
-        <v>-9.36359952131567E-2</v>
-      </c>
-      <c r="BD9" s="8">
-        <v>-1.92530848685795</v>
-      </c>
-      <c r="BF9" s="8">
-        <v>-0.80560859369899596</v>
-      </c>
-      <c r="BG9" s="8">
-        <v>-4.6052482635112399</v>
-      </c>
-    </row>
-    <row r="10" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="Y10" s="19">
+      <c r="AQ9">
+        <v>-4.0211733634489901</v>
+      </c>
+      <c r="AR9">
+        <v>7.9179600361809799</v>
+      </c>
+      <c r="AS9" s="14"/>
+      <c r="AT9">
+        <v>-4.0245359599571202</v>
+      </c>
+      <c r="AU9">
+        <v>8.1274578560828807</v>
+      </c>
+      <c r="AV9" s="14"/>
+      <c r="AW9">
+        <v>-4.0769949089828703</v>
+      </c>
+      <c r="AX9">
+        <v>6.0033053056678698</v>
+      </c>
+      <c r="AY9" s="14"/>
+      <c r="AZ9">
+        <v>-3.6764254205438101</v>
+      </c>
+      <c r="BA9">
+        <v>9.4019348869036907</v>
+      </c>
+      <c r="BC9">
+        <v>-3.7451790811900398</v>
+      </c>
+      <c r="BD9">
+        <v>9.4319212030878994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="Y10" s="14">
         <v>87.014102041254304</v>
       </c>
-      <c r="Z10" s="19">
+      <c r="Z10" s="14">
         <v>8.6540814355319906</v>
       </c>
-      <c r="AB10" s="19">
+      <c r="AB10" s="14">
         <v>149.66515701131101</v>
       </c>
-      <c r="AC10" s="19">
+      <c r="AC10" s="14">
         <v>2.0114190044860401</v>
       </c>
       <c r="AE10" s="2">
@@ -6742,58 +6687,51 @@
       <c r="AL10" s="2">
         <v>36.966470636071698</v>
       </c>
-      <c r="AQ10" s="8">
-        <v>-2.0624267797481002</v>
-      </c>
-      <c r="AR10" s="8">
-        <v>-9.5687567437458405</v>
-      </c>
-      <c r="AS10" s="19"/>
-      <c r="AT10" s="8">
-        <v>-1.1539321809085099</v>
-      </c>
-      <c r="AU10" s="8">
-        <v>-1.1539321809085099</v>
-      </c>
-      <c r="AV10" s="19"/>
-      <c r="AW10" s="8">
-        <v>-1.0526134039017201</v>
-      </c>
-      <c r="AX10" s="8">
-        <v>-5.0672840532429904</v>
-      </c>
-      <c r="AY10" s="19"/>
-      <c r="AZ10" s="8">
-        <v>-1.2108607442208801</v>
-      </c>
-      <c r="BA10" s="8">
-        <v>-8.7494031056407309</v>
-      </c>
-      <c r="BB10" s="19"/>
-      <c r="BC10" s="8">
-        <v>-4.2639596705317501E-2</v>
-      </c>
-      <c r="BD10" s="8">
-        <v>-1.5696454660068999</v>
-      </c>
-      <c r="BF10" s="8">
-        <v>-0.80826056209367703</v>
-      </c>
-      <c r="BG10" s="8">
-        <v>-3.9574976521681098</v>
-      </c>
-    </row>
-    <row r="11" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="Y11" s="19">
+      <c r="AQ10">
+        <v>-3.98573409720301</v>
+      </c>
+      <c r="AR10">
+        <v>7.9410517458879903</v>
+      </c>
+      <c r="AS10" s="14"/>
+      <c r="AT10">
+        <v>-3.9827575435751799</v>
+      </c>
+      <c r="AU10">
+        <v>8.0697435541028995</v>
+      </c>
+      <c r="AV10" s="14"/>
+      <c r="AW10">
+        <v>-4.1203560536534702</v>
+      </c>
+      <c r="AX10">
+        <v>5.9542771455551504</v>
+      </c>
+      <c r="AY10" s="14"/>
+      <c r="AZ10">
+        <v>-3.6701192496529602</v>
+      </c>
+      <c r="BA10">
+        <v>9.2539316714557192</v>
+      </c>
+      <c r="BC10">
+        <v>-3.8139119928634302</v>
+      </c>
+      <c r="BD10">
+        <v>8.8241552023164704</v>
+      </c>
+    </row>
+    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="Y11" s="14">
         <v>97.375990040567501</v>
       </c>
-      <c r="Z11" s="19">
+      <c r="Z11" s="14">
         <v>8.7346798600528004</v>
       </c>
-      <c r="AB11" s="19">
+      <c r="AB11" s="14">
         <v>199.813260640923</v>
       </c>
-      <c r="AC11" s="19">
+      <c r="AC11" s="14">
         <v>1.7241194273326299</v>
       </c>
       <c r="AE11" s="2">
@@ -6814,56 +6752,49 @@
       <c r="AL11" s="2">
         <v>35.7320954530554</v>
       </c>
-      <c r="AQ11" s="8">
-        <v>-2.0299570388200698</v>
-      </c>
-      <c r="AR11" s="8">
-        <v>-9.7336079621089908</v>
-      </c>
-      <c r="AS11" s="19"/>
-      <c r="AT11" s="8">
-        <v>-1.1081796080110899</v>
-      </c>
-      <c r="AU11" s="8">
-        <v>-6.7664089717055402</v>
-      </c>
-      <c r="AV11" s="19"/>
-      <c r="AW11" s="8">
-        <v>-0.98073859195666602</v>
-      </c>
-      <c r="AX11" s="8">
-        <v>-4.7048341801959301</v>
-      </c>
-      <c r="AY11" s="19"/>
-      <c r="AZ11" s="8">
-        <v>-1.1800590095235299</v>
-      </c>
-      <c r="BA11" s="8">
-        <v>-8.0376015110816699</v>
-      </c>
-      <c r="BB11" s="19"/>
-      <c r="BC11" s="8">
-        <v>-2.6988400793745999E-2</v>
-      </c>
-      <c r="BD11" s="8">
-        <v>-1.38081591094805</v>
-      </c>
-      <c r="BF11" s="8">
-        <v>-0.70163200563028605</v>
-      </c>
-      <c r="BG11" s="8">
-        <v>-3.6126569968387101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="Y12" s="19">
+      <c r="AQ11">
+        <v>-4.0757670451767902</v>
+      </c>
+      <c r="AR11">
+        <v>7.4631272832138098</v>
+      </c>
+      <c r="AS11" s="14"/>
+      <c r="AT11">
+        <v>-4.2998502451406804</v>
+      </c>
+      <c r="AU11">
+        <v>6.63695622990197</v>
+      </c>
+      <c r="AV11" s="14"/>
+      <c r="AW11">
+        <v>-4.1985846936482796</v>
+      </c>
+      <c r="AX11">
+        <v>5.5519574558734099</v>
+      </c>
+      <c r="AY11" s="14"/>
+      <c r="AZ11">
+        <v>-3.61364203861825</v>
+      </c>
+      <c r="BA11">
+        <v>9.3398309150851606</v>
+      </c>
+      <c r="BC11">
+        <v>-3.9051158246998998</v>
+      </c>
+      <c r="BD11">
+        <v>8.5773109848569309</v>
+      </c>
+    </row>
+    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="Y12" s="14">
         <v>104.39696065594801</v>
       </c>
-      <c r="Z12" s="19">
+      <c r="Z12" s="14">
         <v>8.0860288909399198</v>
       </c>
-      <c r="AB12" s="19"/>
-      <c r="AC12" s="19"/>
+      <c r="AB12" s="14"/>
+      <c r="AC12" s="14"/>
       <c r="AE12" s="2">
         <v>0.42329894463199502</v>
       </c>
@@ -6882,56 +6813,49 @@
       <c r="AL12" s="2">
         <v>35.879322563487499</v>
       </c>
-      <c r="AQ12" s="8">
-        <v>-1.95195293681877</v>
-      </c>
-      <c r="AR12" s="8">
-        <v>-9.8659924365665308</v>
-      </c>
-      <c r="AS12" s="19"/>
-      <c r="AT12" s="8">
-        <v>-1.11295090856554</v>
-      </c>
-      <c r="AU12" s="8">
-        <v>-6.3029481331296502</v>
-      </c>
-      <c r="AV12" s="19"/>
-      <c r="AW12" s="8">
-        <v>-0.96945840489270796</v>
-      </c>
-      <c r="AX12" s="8">
-        <v>-5.0882635254700403</v>
-      </c>
-      <c r="AY12" s="19"/>
-      <c r="AZ12" s="8">
-        <v>-1.1119092268920501</v>
-      </c>
-      <c r="BA12" s="8">
-        <v>-8.1466240192601305</v>
-      </c>
-      <c r="BB12" s="19"/>
-      <c r="BC12" s="8">
-        <v>0.27981719361032298</v>
-      </c>
-      <c r="BD12" s="8">
-        <v>0.77495971106963601</v>
-      </c>
-      <c r="BF12" s="8">
-        <v>-0.67599570023650901</v>
-      </c>
-      <c r="BG12" s="8">
-        <v>-3.3739386047667201</v>
-      </c>
-    </row>
-    <row r="13" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="Y13" s="19">
+      <c r="AQ12">
+        <v>-4.1619318202551598</v>
+      </c>
+      <c r="AR12">
+        <v>7.0423015302294596</v>
+      </c>
+      <c r="AS12" s="14"/>
+      <c r="AT12">
+        <v>-4.35774241891027</v>
+      </c>
+      <c r="AU12">
+        <v>5.8641476497310201</v>
+      </c>
+      <c r="AV12" s="14"/>
+      <c r="AW12">
+        <v>-4.2215149013997699</v>
+      </c>
+      <c r="AX12">
+        <v>5.3722769795885599</v>
+      </c>
+      <c r="AY12" s="14"/>
+      <c r="AZ12">
+        <v>-3.6119508312228299</v>
+      </c>
+      <c r="BA12">
+        <v>9.2128890466017399</v>
+      </c>
+      <c r="BC12">
+        <v>-3.90410974086618</v>
+      </c>
+      <c r="BD12">
+        <v>8.6968342077076102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="Y13" s="14">
         <v>142.870634699177</v>
       </c>
-      <c r="Z13" s="19">
+      <c r="Z13" s="14">
         <v>4.5758655476614596</v>
       </c>
-      <c r="AB13" s="19"/>
-      <c r="AC13" s="19"/>
+      <c r="AB13" s="14"/>
+      <c r="AC13" s="14"/>
       <c r="AE13" s="2">
         <v>0.47082950566652898</v>
       </c>
@@ -6950,52 +6874,45 @@
       <c r="AL13" s="2">
         <v>36.0090133942292</v>
       </c>
-      <c r="AQ13" s="8">
-        <v>-1.9694831203739001</v>
-      </c>
-      <c r="AR13" s="8">
-        <v>-9.4462534522160908</v>
-      </c>
-      <c r="AS13" s="19"/>
-      <c r="AT13" s="8">
-        <v>-1.0729224191506299</v>
-      </c>
-      <c r="AU13" s="8">
-        <v>-6.4409117341905402</v>
-      </c>
-      <c r="AV13" s="19"/>
-      <c r="AW13" s="19"/>
-      <c r="AX13" s="19"/>
-      <c r="AY13" s="19"/>
-      <c r="AZ13" s="8">
-        <v>-1.02451526844284</v>
-      </c>
-      <c r="BA13" s="8">
-        <v>-8.2093914781896995</v>
-      </c>
-      <c r="BB13" s="19"/>
-      <c r="BC13" s="8">
-        <v>0.306169075201979</v>
-      </c>
-      <c r="BD13" s="8">
-        <v>1.0654447209300599</v>
-      </c>
-      <c r="BF13" s="8">
-        <v>-0.53515913403799997</v>
-      </c>
-      <c r="BG13" s="8">
-        <v>-2.62067053290995</v>
-      </c>
-    </row>
-    <row r="14" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="Y14" s="19">
+      <c r="AQ13">
+        <v>-4.2020348643493701</v>
+      </c>
+      <c r="AR13">
+        <v>6.8133631013169698</v>
+      </c>
+      <c r="AS13" s="14"/>
+      <c r="AT13" s="14"/>
+      <c r="AU13" s="14"/>
+      <c r="AV13" s="14"/>
+      <c r="AW13">
+        <v>-4.2548497782274399</v>
+      </c>
+      <c r="AX13">
+        <v>5.1792565504348902</v>
+      </c>
+      <c r="AY13" s="14"/>
+      <c r="AZ13">
+        <v>-3.7264517501916199</v>
+      </c>
+      <c r="BA13">
+        <v>9.0545239184644899</v>
+      </c>
+      <c r="BC13">
+        <v>-3.7603984462639599</v>
+      </c>
+      <c r="BD13">
+        <v>9.5569156494016898</v>
+      </c>
+    </row>
+    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="Y14" s="14">
         <v>162.50617098456701</v>
       </c>
-      <c r="Z14" s="19">
+      <c r="Z14" s="14">
         <v>3.5872201592650601</v>
       </c>
-      <c r="AB14" s="19"/>
-      <c r="AC14" s="19"/>
+      <c r="AB14" s="14"/>
+      <c r="AC14" s="14"/>
       <c r="AE14" s="2">
         <v>0.50695422009538504</v>
       </c>
@@ -7014,52 +6931,45 @@
       <c r="AL14" s="2">
         <v>35.349521004796202</v>
       </c>
-      <c r="AQ14" s="8">
-        <v>-1.92571580372108</v>
-      </c>
-      <c r="AR14" s="8">
-        <v>-9.1011493172592903</v>
-      </c>
-      <c r="AS14" s="19"/>
-      <c r="AT14" s="8">
-        <v>-0.99019701504388902</v>
-      </c>
-      <c r="AU14" s="8">
-        <v>-5.9782976379178301</v>
-      </c>
-      <c r="AV14" s="19"/>
-      <c r="AW14" s="19"/>
-      <c r="AX14" s="19"/>
-      <c r="AY14" s="19"/>
-      <c r="AZ14" s="8">
-        <v>-1.0794359490835801</v>
-      </c>
-      <c r="BA14" s="8">
-        <v>-7.6980058724391602</v>
-      </c>
-      <c r="BB14" s="19"/>
-      <c r="BC14" s="8">
-        <v>0.32673053329437501</v>
-      </c>
-      <c r="BD14" s="8">
-        <v>1.20334725241051</v>
-      </c>
-      <c r="BF14" s="8">
-        <v>-0.51445197100600204</v>
-      </c>
-      <c r="BG14" s="8">
-        <v>-2.2372668299063401</v>
-      </c>
-    </row>
-    <row r="15" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="Y15" s="19">
+      <c r="AQ14">
+        <v>-4.26390426307605</v>
+      </c>
+      <c r="AR14">
+        <v>6.6558306749259604</v>
+      </c>
+      <c r="AS14" s="14"/>
+      <c r="AT14" s="14"/>
+      <c r="AU14" s="14"/>
+      <c r="AV14" s="14"/>
+      <c r="AW14">
+        <v>-4.28014227578175</v>
+      </c>
+      <c r="AX14">
+        <v>5.0359415012234798</v>
+      </c>
+      <c r="AY14" s="14"/>
+      <c r="AZ14">
+        <v>-3.6958014223150002</v>
+      </c>
+      <c r="BA14">
+        <v>9.0051782625956296</v>
+      </c>
+      <c r="BC14">
+        <v>-3.6879078477215801</v>
+      </c>
+      <c r="BD14">
+        <v>9.9432504987057904</v>
+      </c>
+    </row>
+    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="Y15" s="14">
         <v>182.702998561892</v>
       </c>
-      <c r="Z15" s="19">
+      <c r="Z15" s="14">
         <v>2.56047564875829</v>
       </c>
-      <c r="AB15" s="19"/>
-      <c r="AC15" s="19"/>
+      <c r="AB15" s="14"/>
+      <c r="AC15" s="14"/>
       <c r="AE15" s="2">
         <v>0.56691117695895799</v>
       </c>
@@ -7078,52 +6988,45 @@
       <c r="AL15" s="2">
         <v>34.309850848255302</v>
       </c>
-      <c r="AQ15" s="8">
-        <v>-1.93511206842088</v>
-      </c>
-      <c r="AR15" s="8">
-        <v>-9.4630397748058908</v>
-      </c>
-      <c r="AS15" s="19"/>
-      <c r="AT15" s="8">
-        <v>-0.97948216384299203</v>
-      </c>
-      <c r="AU15" s="8">
-        <v>-5.6887671645889997</v>
-      </c>
-      <c r="AV15" s="19"/>
-      <c r="AW15" s="19"/>
-      <c r="AX15" s="19"/>
-      <c r="AY15" s="19"/>
-      <c r="AZ15" s="8">
-        <v>-1.0497474485634699</v>
-      </c>
-      <c r="BA15" s="8">
-        <v>-7.8066561746617102</v>
-      </c>
-      <c r="BB15" s="19"/>
-      <c r="BC15" s="8">
-        <v>0.35971486997151902</v>
-      </c>
-      <c r="BD15" s="8">
-        <v>1.71909159897549</v>
-      </c>
-      <c r="BF15" s="8">
-        <v>-0.440337976595155</v>
-      </c>
-      <c r="BG15" s="8">
-        <v>-1.36386981306695</v>
-      </c>
-    </row>
-    <row r="16" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="Y16" s="19">
+      <c r="AQ15">
+        <v>-4.31767705863132</v>
+      </c>
+      <c r="AR15">
+        <v>6.3299157626865004</v>
+      </c>
+      <c r="AS15" s="14"/>
+      <c r="AT15" s="14"/>
+      <c r="AU15" s="14"/>
+      <c r="AV15" s="14"/>
+      <c r="AW15">
+        <v>-4.2479890296160603</v>
+      </c>
+      <c r="AX15">
+        <v>4.7933818026517798</v>
+      </c>
+      <c r="AY15" s="14"/>
+      <c r="AZ15">
+        <v>-3.6704694038557499</v>
+      </c>
+      <c r="BA15">
+        <v>8.9287802516112595</v>
+      </c>
+      <c r="BC15">
+        <v>-3.9279277084412398</v>
+      </c>
+      <c r="BD15">
+        <v>8.2970002649992001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="Y16" s="14">
         <v>202.88372791860701</v>
       </c>
-      <c r="Z16" s="19">
+      <c r="Z16" s="14">
         <v>2.1084376140290599</v>
       </c>
-      <c r="AB16" s="19"/>
-      <c r="AC16" s="19"/>
+      <c r="AB16" s="14"/>
+      <c r="AC16" s="14"/>
       <c r="AE16" s="2">
         <v>0.55974749182729799</v>
       </c>
@@ -7136,48 +7039,45 @@
       <c r="AL16" s="2">
         <v>34.308871922151297</v>
       </c>
-      <c r="AQ16" s="8">
-        <v>-1.90266390605429</v>
-      </c>
-      <c r="AR16" s="8">
-        <v>-9.7019324321229803</v>
-      </c>
-      <c r="AS16" s="19"/>
-      <c r="AT16" s="8">
-        <v>-0.945196750261312</v>
-      </c>
-      <c r="AU16" s="8">
-        <v>-5.89184287472004</v>
-      </c>
-      <c r="AV16" s="19"/>
-      <c r="AW16" s="19"/>
-      <c r="AX16" s="19"/>
-      <c r="AY16" s="19"/>
-      <c r="AZ16" s="8">
-        <v>-1.0216898868683799</v>
-      </c>
-      <c r="BA16" s="8">
-        <v>-7.5127995724655898</v>
-      </c>
-      <c r="BB16" s="19"/>
-      <c r="BC16" s="19"/>
-      <c r="BD16" s="19"/>
-      <c r="BF16" s="8">
-        <v>-0.379944757157893</v>
-      </c>
-      <c r="BG16" s="8">
-        <v>-1.2701253877815799</v>
-      </c>
-    </row>
-    <row r="17" spans="25:59" x14ac:dyDescent="0.25">
-      <c r="Y17" s="19">
+      <c r="AQ16">
+        <v>-4.3550899132307697</v>
+      </c>
+      <c r="AR16">
+        <v>6.3092593368657397</v>
+      </c>
+      <c r="AS16" s="14"/>
+      <c r="AT16" s="14"/>
+      <c r="AU16" s="14"/>
+      <c r="AV16" s="14"/>
+      <c r="AW16">
+        <v>-4.3036491493862101</v>
+      </c>
+      <c r="AX16">
+        <v>4.4003004136636701</v>
+      </c>
+      <c r="AY16" s="14"/>
+      <c r="AZ16">
+        <v>-3.7116631471967598</v>
+      </c>
+      <c r="BA16">
+        <v>8.8509140217279203</v>
+      </c>
+      <c r="BC16">
+        <v>-4.2123543406781998</v>
+      </c>
+      <c r="BD16">
+        <v>6.95289451207322</v>
+      </c>
+    </row>
+    <row r="17" spans="25:56" x14ac:dyDescent="0.25">
+      <c r="Y17" s="14">
         <v>222.78112859258599</v>
       </c>
-      <c r="Z17" s="19">
+      <c r="Z17" s="14">
         <v>1.7712335529845999</v>
       </c>
-      <c r="AB17" s="19"/>
-      <c r="AC17" s="19"/>
+      <c r="AB17" s="14"/>
+      <c r="AC17" s="14"/>
       <c r="AE17" s="2">
         <v>0.55375812032203398</v>
       </c>
@@ -7190,48 +7090,41 @@
       <c r="AL17" s="2">
         <v>33.333135767022299</v>
       </c>
-      <c r="AQ17" s="8">
-        <v>-1.85317587300094</v>
-      </c>
-      <c r="AR17" s="8">
-        <v>-8.8550458239930698</v>
-      </c>
-      <c r="AS17" s="19"/>
-      <c r="AT17" s="8">
-        <v>-0.94101737797113405</v>
-      </c>
-      <c r="AU17" s="8">
-        <v>-5.5805265924133201</v>
-      </c>
-      <c r="AV17" s="19"/>
-      <c r="AW17" s="19"/>
-      <c r="AX17" s="19"/>
-      <c r="AY17" s="19"/>
-      <c r="AZ17" s="8">
-        <v>-0.90371526150170101</v>
-      </c>
-      <c r="BA17" s="8">
-        <v>-7.62230425654149</v>
-      </c>
-      <c r="BB17" s="19"/>
-      <c r="BC17" s="19"/>
-      <c r="BD17" s="19"/>
-      <c r="BF17" s="8">
-        <v>-0.370152450915475</v>
-      </c>
-      <c r="BG17" s="8">
-        <v>-1.7858846730539299</v>
-      </c>
-    </row>
-    <row r="18" spans="25:59" x14ac:dyDescent="0.25">
-      <c r="Y18" s="19">
+      <c r="AQ17">
+        <v>-4.3705246829828601</v>
+      </c>
+      <c r="AR17">
+        <v>6.0511192449245197</v>
+      </c>
+      <c r="AS17" s="14"/>
+      <c r="AT17" s="14"/>
+      <c r="AU17" s="14"/>
+      <c r="AV17" s="14"/>
+      <c r="AW17">
+        <v>-4.3592595708158299</v>
+      </c>
+      <c r="AX17">
+        <v>4.4223803356534503</v>
+      </c>
+      <c r="AY17" s="14"/>
+      <c r="AZ17">
+        <v>-3.73853430439459</v>
+      </c>
+      <c r="BA17">
+        <v>8.9349737727138194</v>
+      </c>
+      <c r="BC17" s="8"/>
+      <c r="BD17" s="8"/>
+    </row>
+    <row r="18" spans="25:56" x14ac:dyDescent="0.25">
+      <c r="Y18" s="14">
         <v>242.672089978321</v>
       </c>
-      <c r="Z18" s="19">
+      <c r="Z18" s="14">
         <v>1.6639120822511699</v>
       </c>
-      <c r="AB18" s="19"/>
-      <c r="AC18" s="19"/>
+      <c r="AB18" s="14"/>
+      <c r="AC18" s="14"/>
       <c r="AE18" s="2">
         <v>0.59188425206134399</v>
       </c>
@@ -7244,42 +7137,35 @@
       <c r="AL18" s="2">
         <v>30.927880573458499</v>
       </c>
-      <c r="AQ18" s="8">
-        <v>-1.82624462951014</v>
-      </c>
-      <c r="AR18" s="8">
-        <v>-8.8964406976960397</v>
-      </c>
-      <c r="AS18" s="19"/>
-      <c r="AT18" s="8">
-        <v>-0.90672563360587899</v>
-      </c>
-      <c r="AU18" s="8">
-        <v>-5.7618798014022099</v>
-      </c>
-      <c r="AV18" s="19"/>
-      <c r="AW18" s="19"/>
-      <c r="AX18" s="19"/>
-      <c r="AY18" s="19"/>
-      <c r="AZ18" s="8">
-        <v>-0.78106550374934203</v>
-      </c>
-      <c r="BA18" s="8">
-        <v>-6.6869253116443703</v>
-      </c>
-      <c r="BB18" s="19"/>
-      <c r="BC18" s="19"/>
-      <c r="BD18" s="19"/>
-      <c r="BF18" s="8">
-        <v>-0.29369713679197801</v>
-      </c>
-      <c r="BG18" s="8">
-        <v>-0.189322266377554</v>
-      </c>
-    </row>
-    <row r="19" spans="25:59" x14ac:dyDescent="0.25">
-      <c r="AB19" s="19"/>
-      <c r="AC19" s="19"/>
+      <c r="AQ18">
+        <v>-4.4185726429303296</v>
+      </c>
+      <c r="AR18">
+        <v>5.87158228913286</v>
+      </c>
+      <c r="AS18" s="14"/>
+      <c r="AT18" s="14"/>
+      <c r="AU18" s="14"/>
+      <c r="AV18" s="14"/>
+      <c r="AW18">
+        <v>-4.3573648220137597</v>
+      </c>
+      <c r="AX18">
+        <v>4.2986024396378504</v>
+      </c>
+      <c r="AY18" s="14"/>
+      <c r="AZ18">
+        <v>-3.7999373896031501</v>
+      </c>
+      <c r="BA18">
+        <v>8.5142024875639706</v>
+      </c>
+      <c r="BC18" s="8"/>
+      <c r="BD18" s="8"/>
+    </row>
+    <row r="19" spans="25:56" x14ac:dyDescent="0.25">
+      <c r="AB19" s="14"/>
+      <c r="AC19" s="14"/>
       <c r="AE19" s="2">
         <v>0.59648602383278104</v>
       </c>
@@ -7292,605 +7178,484 @@
       <c r="AL19" s="2">
         <v>29.591595807409998</v>
       </c>
-      <c r="AQ19" s="8">
-        <v>-1.7732201099979501</v>
-      </c>
-      <c r="AR19" s="8">
-        <v>-8.6666020451180596</v>
-      </c>
-      <c r="AS19" s="19"/>
-      <c r="AT19" s="8">
-        <v>-0.90823658061914203</v>
-      </c>
-      <c r="AU19" s="8">
-        <v>-5.3346547853144397</v>
-      </c>
-      <c r="AV19" s="19"/>
-      <c r="AW19" s="19"/>
-      <c r="AX19" s="19"/>
-      <c r="AY19" s="19"/>
-      <c r="AZ19" s="19"/>
-      <c r="BA19" s="19"/>
-      <c r="BB19" s="19"/>
-      <c r="BC19" s="19"/>
-      <c r="BD19" s="19"/>
-      <c r="BF19" s="8">
-        <v>-0.25022556503134902</v>
-      </c>
-      <c r="BG19" s="8">
-        <v>0.32592156201089401</v>
-      </c>
-    </row>
-    <row r="20" spans="25:59" x14ac:dyDescent="0.25">
+      <c r="AQ19">
+        <v>-4.4854629167333604</v>
+      </c>
+      <c r="AR19">
+        <v>5.7883042776659801</v>
+      </c>
+      <c r="AS19" s="14"/>
+      <c r="AT19" s="14"/>
+      <c r="AU19" s="14"/>
+      <c r="AV19" s="14"/>
+      <c r="AW19">
+        <v>-4.4377626156484498</v>
+      </c>
+      <c r="AX19">
+        <v>3.7811553789330299</v>
+      </c>
+      <c r="AY19" s="14"/>
+      <c r="AZ19">
+        <v>-3.7654490257612099</v>
+      </c>
+      <c r="BA19">
+        <v>8.4533979738514304</v>
+      </c>
+      <c r="BC19" s="8"/>
+      <c r="BD19" s="8"/>
+    </row>
+    <row r="20" spans="25:56" x14ac:dyDescent="0.25">
       <c r="AE20" s="2">
         <v>0.67760046653958905</v>
       </c>
       <c r="AF20" s="2">
         <v>42.207721914506301</v>
       </c>
-      <c r="AQ20" s="8">
-        <v>-1.76025139457024</v>
-      </c>
-      <c r="AR20" s="8">
-        <v>-8.7983571448668307</v>
-      </c>
-      <c r="AS20" s="19"/>
-      <c r="AT20" s="8">
-        <v>-0.86985620519495299</v>
-      </c>
-      <c r="AU20" s="8">
-        <v>-5.5160475617006801</v>
-      </c>
-      <c r="AV20" s="19"/>
-      <c r="AW20" s="19"/>
-      <c r="AX20" s="19"/>
-      <c r="AY20" s="19"/>
-      <c r="AZ20" s="19"/>
-      <c r="BA20" s="19"/>
-      <c r="BB20" s="19"/>
-      <c r="BC20" s="19"/>
-      <c r="BD20" s="19"/>
-      <c r="BF20" s="8">
-        <v>-0.15124593054114399</v>
-      </c>
-      <c r="BG20" s="8">
-        <v>1.23052090222239</v>
-      </c>
-    </row>
-    <row r="21" spans="25:59" x14ac:dyDescent="0.25">
+      <c r="AQ20">
+        <v>-4.5219600805864602</v>
+      </c>
+      <c r="AR20">
+        <v>5.8222025596181597</v>
+      </c>
+      <c r="AS20" s="14"/>
+      <c r="AT20" s="14"/>
+      <c r="AU20" s="14"/>
+      <c r="AV20" s="14"/>
+      <c r="AW20" s="14"/>
+      <c r="AX20" s="14"/>
+      <c r="AY20" s="14"/>
+      <c r="AZ20">
+        <v>-3.7309680200800801</v>
+      </c>
+      <c r="BA20">
+        <v>8.3983650792589799</v>
+      </c>
+      <c r="BC20" s="8"/>
+      <c r="BD20" s="8"/>
+    </row>
+    <row r="21" spans="25:56" x14ac:dyDescent="0.25">
       <c r="AE21" s="2">
         <v>0.87243856571592804</v>
       </c>
       <c r="AF21" s="2">
         <v>37.466725156371503</v>
       </c>
-      <c r="AQ21" s="8">
-        <v>-1.72666796010991</v>
-      </c>
-      <c r="AR21" s="8">
-        <v>-8.3297517099135092</v>
-      </c>
-      <c r="AS21" s="19"/>
-      <c r="AT21" s="8">
-        <v>-0.868943517229539</v>
-      </c>
-      <c r="AU21" s="8">
-        <v>-5.1902179580479899</v>
-      </c>
-      <c r="AV21" s="19"/>
-      <c r="AW21" s="19"/>
-      <c r="AX21" s="19"/>
-      <c r="AY21" s="19"/>
-      <c r="AZ21" s="19"/>
-      <c r="BA21" s="19"/>
-      <c r="BB21" s="19"/>
-      <c r="BC21" s="19"/>
-      <c r="BD21" s="19"/>
-    </row>
-    <row r="22" spans="25:59" x14ac:dyDescent="0.25">
+      <c r="AQ21">
+        <v>-4.4508255757451298</v>
+      </c>
+      <c r="AR21">
+        <v>5.6676055200543196</v>
+      </c>
+      <c r="AS21" s="14"/>
+      <c r="AT21" s="14"/>
+      <c r="AU21" s="14"/>
+      <c r="AV21" s="14"/>
+      <c r="AW21" s="14"/>
+      <c r="AX21" s="14"/>
+      <c r="AY21" s="14"/>
+      <c r="AZ21">
+        <v>-3.7813230142443301</v>
+      </c>
+      <c r="BA21">
+        <v>8.3087530981838693</v>
+      </c>
+    </row>
+    <row r="22" spans="25:56" x14ac:dyDescent="0.25">
       <c r="AE22" s="2">
         <v>0.82473811981675205</v>
       </c>
       <c r="AF22" s="2">
         <v>44.287577671041099</v>
       </c>
-      <c r="AQ22" s="8">
-        <v>-1.64311337258169</v>
-      </c>
-      <c r="AR22" s="8">
-        <v>-8.5444583962790404</v>
-      </c>
-      <c r="AS22" s="19"/>
-      <c r="AT22" s="8">
-        <v>-0.83627878424309099</v>
-      </c>
-      <c r="AU22" s="8">
-        <v>-5.3425920052217499</v>
-      </c>
-      <c r="AV22" s="19"/>
-      <c r="AW22" s="19"/>
-      <c r="AX22" s="19"/>
-      <c r="AY22" s="19"/>
-      <c r="AZ22" s="19"/>
-      <c r="BA22" s="19"/>
-      <c r="BB22" s="19"/>
-      <c r="BC22" s="19"/>
-      <c r="BD22" s="19"/>
-    </row>
-    <row r="23" spans="25:59" x14ac:dyDescent="0.25">
+      <c r="AQ22">
+        <v>-4.5477676630322703</v>
+      </c>
+      <c r="AR22">
+        <v>5.1994439365312104</v>
+      </c>
+      <c r="AS22" s="14"/>
+      <c r="AT22" s="14"/>
+      <c r="AU22" s="14"/>
+      <c r="AV22" s="14"/>
+      <c r="AW22" s="14"/>
+      <c r="AX22" s="14"/>
+      <c r="AY22" s="14"/>
+      <c r="AZ22">
+        <v>-3.80663050550086</v>
+      </c>
+      <c r="BA22">
+        <v>8.3659123787679395</v>
+      </c>
+    </row>
+    <row r="23" spans="25:56" x14ac:dyDescent="0.25">
       <c r="AE23" s="2">
         <v>0.91037745209347998</v>
       </c>
       <c r="AF23" s="2">
         <v>42.942201146271501</v>
       </c>
-      <c r="AQ23" s="8">
-        <v>-1.6272495334936099</v>
-      </c>
-      <c r="AR23" s="8">
-        <v>-8.3060332744598995</v>
-      </c>
-      <c r="AS23" s="19"/>
-      <c r="AT23" s="8">
-        <v>-0.82962724096682805</v>
-      </c>
-      <c r="AU23" s="8">
-        <v>-4.966131959927</v>
-      </c>
-      <c r="AV23" s="19"/>
-      <c r="AW23" s="19"/>
-      <c r="AX23" s="19"/>
-      <c r="AY23" s="19"/>
-      <c r="AZ23" s="19"/>
-      <c r="BA23" s="19"/>
-      <c r="BB23" s="19"/>
-      <c r="BC23" s="19"/>
-      <c r="BD23" s="19"/>
-    </row>
-    <row r="24" spans="25:59" x14ac:dyDescent="0.25">
+      <c r="AQ23">
+        <v>-4.6097634678574</v>
+      </c>
+      <c r="AR23">
+        <v>5.1410623540798897</v>
+      </c>
+      <c r="AS23" s="14"/>
+      <c r="AT23" s="14"/>
+      <c r="AU23" s="14"/>
+      <c r="AV23" s="14"/>
+      <c r="AW23" s="14"/>
+      <c r="AX23" s="14"/>
+      <c r="AY23" s="14"/>
+      <c r="AZ23">
+        <v>-3.8647836228132699</v>
+      </c>
+      <c r="BA23">
+        <v>7.7951465008129102</v>
+      </c>
+    </row>
+    <row r="24" spans="25:56" x14ac:dyDescent="0.25">
       <c r="AE24" s="2">
         <v>0.99234715598221002</v>
       </c>
       <c r="AF24" s="2">
         <v>38.024205768125398</v>
       </c>
-      <c r="AQ24" s="8">
-        <v>-1.5603511977820399</v>
-      </c>
-      <c r="AR24" s="8">
-        <v>-8.2902269782023303</v>
-      </c>
-      <c r="AS24" s="19"/>
-      <c r="AT24" s="8">
-        <v>-0.80186253446752498</v>
-      </c>
-      <c r="AU24" s="8">
-        <v>-5.0967360250818103</v>
-      </c>
-      <c r="AV24" s="19"/>
-      <c r="AW24" s="19"/>
-      <c r="AX24" s="19"/>
-      <c r="AY24" s="19"/>
-      <c r="AZ24" s="19"/>
-      <c r="BA24" s="19"/>
-      <c r="BB24" s="19"/>
-      <c r="BC24" s="19"/>
-      <c r="BD24" s="19"/>
-    </row>
-    <row r="25" spans="25:59" x14ac:dyDescent="0.25">
+      <c r="AQ24">
+        <v>-4.67361909554739</v>
+      </c>
+      <c r="AR24">
+        <v>4.99588029596908</v>
+      </c>
+      <c r="AS24" s="14"/>
+      <c r="AT24" s="14"/>
+      <c r="AU24" s="14"/>
+      <c r="AV24" s="14"/>
+      <c r="AW24" s="14"/>
+      <c r="AX24" s="14"/>
+      <c r="AY24" s="14"/>
+      <c r="AZ24">
+        <v>-3.8776455572666002</v>
+      </c>
+      <c r="BA24">
+        <v>7.6871227172231196</v>
+      </c>
+    </row>
+    <row r="25" spans="25:56" x14ac:dyDescent="0.25">
       <c r="AE25" s="2">
         <v>0.98709097296093395</v>
       </c>
       <c r="AF25" s="2">
         <v>40.943798486254899</v>
       </c>
-      <c r="AQ25" s="8">
-        <v>-1.5035576228709999</v>
-      </c>
-      <c r="AR25" s="8">
-        <v>-7.8794341057837904</v>
-      </c>
-      <c r="AS25" s="19"/>
-      <c r="AT25" s="8">
-        <v>-0.79928485042185404</v>
-      </c>
-      <c r="AU25" s="8">
-        <v>-4.66955057639138</v>
-      </c>
-      <c r="AV25" s="19"/>
-      <c r="AW25" s="19"/>
-      <c r="AX25" s="19"/>
-      <c r="AY25" s="19"/>
-      <c r="AZ25" s="19"/>
-      <c r="BA25" s="19"/>
-      <c r="BB25" s="19"/>
-      <c r="BC25" s="19"/>
-      <c r="BD25" s="19"/>
-    </row>
-    <row r="26" spans="25:59" x14ac:dyDescent="0.25">
+      <c r="AQ25">
+        <v>-4.6389785944066899</v>
+      </c>
+      <c r="AR25">
+        <v>4.8727027672589296</v>
+      </c>
+      <c r="AS25" s="14"/>
+      <c r="AT25" s="14"/>
+      <c r="AU25" s="14"/>
+      <c r="AV25" s="14"/>
+      <c r="AW25" s="14"/>
+      <c r="AX25" s="14"/>
+      <c r="AY25" s="14"/>
+      <c r="AZ25" s="14"/>
+      <c r="BA25" s="14"/>
+    </row>
+    <row r="26" spans="25:56" x14ac:dyDescent="0.25">
       <c r="AE26" s="2">
         <v>1.0390150851856901</v>
       </c>
       <c r="AF26" s="2">
         <v>36.6241521329273</v>
       </c>
-      <c r="AQ26" s="8">
-        <v>-1.5545417695177901</v>
-      </c>
-      <c r="AR26" s="8">
-        <v>-7.48405192266301</v>
-      </c>
-      <c r="AS26" s="19"/>
-      <c r="AT26" s="8">
-        <v>-0.93270294887580496</v>
-      </c>
-      <c r="AU26" s="8">
-        <v>-5.1099515357948802</v>
-      </c>
-      <c r="AV26" s="19"/>
-      <c r="AW26" s="19"/>
-      <c r="AX26" s="19"/>
-      <c r="AY26" s="19"/>
-      <c r="AZ26" s="19"/>
-      <c r="BA26" s="19"/>
-      <c r="BB26" s="19"/>
-      <c r="BC26" s="19"/>
-      <c r="BD26" s="19"/>
-    </row>
-    <row r="27" spans="25:59" x14ac:dyDescent="0.25">
+      <c r="AQ26">
+        <v>-4.7008416728284397</v>
+      </c>
+      <c r="AR26">
+        <v>4.7102127986709297</v>
+      </c>
+      <c r="AS26" s="14"/>
+      <c r="AT26" s="14"/>
+      <c r="AU26" s="14"/>
+      <c r="AV26" s="14"/>
+      <c r="AW26" s="14"/>
+      <c r="AX26" s="14"/>
+      <c r="AY26" s="14"/>
+      <c r="AZ26" s="14"/>
+      <c r="BA26" s="14"/>
+    </row>
+    <row r="27" spans="25:56" x14ac:dyDescent="0.25">
       <c r="AE27" s="2">
         <v>1.03874087695692</v>
       </c>
       <c r="AF27" s="2">
         <v>40.526923183051501</v>
       </c>
-      <c r="AQ27" s="8">
-        <v>-1.4264226573723</v>
-      </c>
-      <c r="AR27" s="8">
-        <v>-7.8061389254131104</v>
-      </c>
-      <c r="AS27" s="19"/>
-      <c r="AT27" s="8">
-        <v>-0.97766522895693098</v>
-      </c>
-      <c r="AU27" s="8">
-        <v>-5.0660712921398003</v>
-      </c>
-      <c r="AV27" s="19"/>
-      <c r="AW27" s="19"/>
-      <c r="AX27" s="19"/>
-      <c r="AY27" s="19"/>
-      <c r="AZ27" s="19"/>
-      <c r="BA27" s="19"/>
-      <c r="BB27" s="19"/>
-      <c r="BC27" s="19"/>
-      <c r="BD27" s="19"/>
-    </row>
-    <row r="28" spans="25:59" x14ac:dyDescent="0.25">
+      <c r="AQ27">
+        <v>-4.7626320677435796</v>
+      </c>
+      <c r="AR27">
+        <v>4.4907110948176197</v>
+      </c>
+      <c r="AS27" s="14"/>
+      <c r="AT27" s="14"/>
+      <c r="AU27" s="14"/>
+      <c r="AV27" s="14"/>
+      <c r="AW27" s="14"/>
+      <c r="AX27" s="14"/>
+      <c r="AY27" s="14"/>
+      <c r="AZ27" s="14"/>
+      <c r="BA27" s="14"/>
+    </row>
+    <row r="28" spans="25:56" x14ac:dyDescent="0.25">
       <c r="AE28" s="2">
         <v>1.05393369380095</v>
       </c>
       <c r="AF28" s="2">
         <v>39.3739406174343</v>
       </c>
-      <c r="AQ28" s="8">
-        <v>-1.44863658756969</v>
-      </c>
-      <c r="AR28" s="8">
-        <v>-7.5179842105333403</v>
-      </c>
-      <c r="AS28" s="19"/>
-      <c r="AT28" s="8">
-        <v>-0.82526849647535505</v>
-      </c>
-      <c r="AU28" s="8">
-        <v>-4.0393448119261901</v>
-      </c>
-      <c r="AV28" s="19"/>
-      <c r="AW28" s="19"/>
-      <c r="AX28" s="19"/>
-      <c r="AY28" s="19"/>
-      <c r="AZ28" s="19"/>
-      <c r="BA28" s="19"/>
-      <c r="BB28" s="19"/>
-      <c r="BC28" s="19"/>
-      <c r="BD28" s="19"/>
-    </row>
-    <row r="29" spans="25:59" x14ac:dyDescent="0.25">
+      <c r="AQ28">
+        <v>-4.8098433407562302</v>
+      </c>
+      <c r="AR28">
+        <v>4.4276981242612097</v>
+      </c>
+      <c r="AS28" s="14"/>
+      <c r="AT28" s="14"/>
+      <c r="AU28" s="14"/>
+      <c r="AV28" s="14"/>
+      <c r="AW28" s="14"/>
+      <c r="AX28" s="14"/>
+      <c r="AY28" s="14"/>
+      <c r="AZ28" s="14"/>
+      <c r="BA28" s="14"/>
+    </row>
+    <row r="29" spans="25:56" x14ac:dyDescent="0.25">
       <c r="AE29" s="2">
         <v>1.13135917130162</v>
       </c>
       <c r="AF29" s="2">
         <v>38.387547430343602</v>
       </c>
-      <c r="AQ29" s="8">
-        <v>-1.39657471165969</v>
-      </c>
-      <c r="AR29" s="8">
-        <v>-7.4033121385942202</v>
-      </c>
-      <c r="AS29" s="19"/>
-      <c r="AT29" s="8">
-        <v>-0.792443383638337</v>
-      </c>
-      <c r="AU29" s="8">
-        <v>-3.6414154968323098</v>
-      </c>
-      <c r="AV29" s="19"/>
-      <c r="AW29" s="19"/>
-      <c r="AX29" s="19"/>
-      <c r="AY29" s="19"/>
-      <c r="AZ29" s="19"/>
-      <c r="BA29" s="19"/>
-      <c r="BB29" s="19"/>
-      <c r="BC29" s="19"/>
-      <c r="BD29" s="19"/>
-    </row>
-    <row r="30" spans="25:59" x14ac:dyDescent="0.25">
+      <c r="AQ29">
+        <v>-4.8352945794413396</v>
+      </c>
+      <c r="AR29">
+        <v>4.2982366933803204</v>
+      </c>
+      <c r="AS29" s="14"/>
+      <c r="AT29" s="14"/>
+      <c r="AU29" s="14"/>
+      <c r="AV29" s="14"/>
+      <c r="AW29" s="14"/>
+      <c r="AX29" s="14"/>
+      <c r="AY29" s="14"/>
+      <c r="AZ29" s="14"/>
+      <c r="BA29" s="14"/>
+    </row>
+    <row r="30" spans="25:56" x14ac:dyDescent="0.25">
       <c r="AE30" s="2">
         <v>1.1828430795116101</v>
       </c>
       <c r="AF30" s="2">
         <v>36.756827942010098</v>
       </c>
-      <c r="AQ30" s="8">
-        <v>-1.3408420826862999</v>
-      </c>
-      <c r="AR30" s="8">
-        <v>-7.4449857353825104</v>
-      </c>
-      <c r="AS30" s="19"/>
-      <c r="AT30" s="8">
-        <v>-0.77208252853014203</v>
-      </c>
-      <c r="AU30" s="8">
-        <v>-3.9240058486669001</v>
-      </c>
-      <c r="AV30" s="19"/>
-      <c r="AW30" s="19"/>
-      <c r="AX30" s="19"/>
-      <c r="AY30" s="19"/>
-      <c r="AZ30" s="19"/>
-      <c r="BA30" s="19"/>
-      <c r="BB30" s="19"/>
-      <c r="BC30" s="19"/>
-      <c r="BD30" s="19"/>
-    </row>
-    <row r="31" spans="25:59" x14ac:dyDescent="0.25">
+      <c r="AQ30">
+        <v>-4.8764112790082104</v>
+      </c>
+      <c r="AR30">
+        <v>4.0915854607481297</v>
+      </c>
+      <c r="AS30" s="14"/>
+      <c r="AT30" s="14"/>
+      <c r="AU30" s="14"/>
+      <c r="AV30" s="14"/>
+      <c r="AW30" s="14"/>
+      <c r="AX30" s="14"/>
+      <c r="AY30" s="14"/>
+      <c r="AZ30" s="14"/>
+      <c r="BA30" s="14"/>
+    </row>
+    <row r="31" spans="25:56" x14ac:dyDescent="0.25">
       <c r="AE31" s="2">
         <v>1.28352582735847</v>
       </c>
       <c r="AF31" s="2">
         <v>34.5095811935578</v>
       </c>
-      <c r="AQ31" s="8">
-        <v>-1.24586044806463</v>
-      </c>
-      <c r="AR31" s="8">
-        <v>-6.7054884347044297</v>
-      </c>
-      <c r="AS31" s="19"/>
-      <c r="AT31" s="8">
-        <v>-0.74738192128119996</v>
-      </c>
-      <c r="AU31" s="8">
-        <v>-3.3449765559271301</v>
-      </c>
-      <c r="AV31" s="19"/>
-      <c r="AW31" s="19"/>
-      <c r="AX31" s="19"/>
-      <c r="AY31" s="19"/>
-      <c r="AZ31" s="19"/>
-      <c r="BA31" s="19"/>
-      <c r="BB31" s="19"/>
-      <c r="BC31" s="19"/>
-      <c r="BD31" s="19"/>
-    </row>
-    <row r="32" spans="25:59" x14ac:dyDescent="0.25">
+      <c r="AQ31">
+        <v>-4.9342070949294996</v>
+      </c>
+      <c r="AR31">
+        <v>3.83003162264496</v>
+      </c>
+      <c r="AS31" s="14"/>
+      <c r="AT31" s="14"/>
+      <c r="AU31" s="14"/>
+      <c r="AV31" s="14"/>
+      <c r="AW31" s="14"/>
+      <c r="AX31" s="14"/>
+      <c r="AY31" s="14"/>
+      <c r="AZ31" s="14"/>
+      <c r="BA31" s="14"/>
+    </row>
+    <row r="32" spans="25:56" x14ac:dyDescent="0.25">
       <c r="AE32" s="2">
         <v>1.3013272994976799</v>
       </c>
       <c r="AF32" s="2">
         <v>34.708634304916202</v>
       </c>
-      <c r="AQ32" s="8">
-        <v>-1.27829182710565</v>
-      </c>
-      <c r="AR32" s="8">
-        <v>-6.4090079915342697</v>
-      </c>
-      <c r="AS32" s="19"/>
-      <c r="AT32" s="8">
-        <v>-0.71723367476586397</v>
-      </c>
-      <c r="AU32" s="8">
-        <v>-3.7145518740839298</v>
-      </c>
-      <c r="AV32" s="19"/>
-      <c r="AW32" s="19"/>
-      <c r="AX32" s="19"/>
-      <c r="AY32" s="19"/>
-      <c r="AZ32" s="19"/>
-      <c r="BA32" s="19"/>
-      <c r="BB32" s="19"/>
-      <c r="BC32" s="19"/>
-      <c r="BD32" s="19"/>
-    </row>
-    <row r="33" spans="31:56" x14ac:dyDescent="0.25">
+      <c r="AQ32">
+        <v>-4.9478168034937902</v>
+      </c>
+      <c r="AR32">
+        <v>3.6859584884466399</v>
+      </c>
+      <c r="AS32" s="14"/>
+      <c r="AT32" s="14"/>
+      <c r="AU32" s="14"/>
+      <c r="AV32" s="14"/>
+      <c r="AW32" s="14"/>
+      <c r="AX32" s="14"/>
+      <c r="AY32" s="14"/>
+      <c r="AZ32" s="14"/>
+      <c r="BA32" s="14"/>
+    </row>
+    <row r="33" spans="31:53" x14ac:dyDescent="0.25">
       <c r="AE33" s="2">
         <v>1.3152614900655699</v>
       </c>
       <c r="AF33" s="2">
         <v>36.167784541143</v>
       </c>
-      <c r="AQ33" s="8">
-        <v>-1.2326999232018701</v>
-      </c>
-      <c r="AR33" s="8">
-        <v>-6.1790974104181497</v>
-      </c>
-      <c r="AS33" s="19"/>
-      <c r="AT33" s="8">
-        <v>-0.66398228872370901</v>
-      </c>
-      <c r="AU33" s="8">
-        <v>-3.3747470656891498</v>
-      </c>
-      <c r="AV33" s="19"/>
-      <c r="AW33" s="19"/>
-      <c r="AX33" s="19"/>
-      <c r="AY33" s="19"/>
-      <c r="AZ33" s="19"/>
-      <c r="BA33" s="19"/>
-      <c r="BB33" s="19"/>
-      <c r="BC33" s="19"/>
-      <c r="BD33" s="19"/>
-    </row>
-    <row r="34" spans="31:56" x14ac:dyDescent="0.25">
+      <c r="AQ33">
+        <v>-5.0068348449501796</v>
+      </c>
+      <c r="AR33">
+        <v>3.6102907391242498</v>
+      </c>
+      <c r="AS33" s="14"/>
+      <c r="AT33" s="14"/>
+      <c r="AU33" s="14"/>
+      <c r="AV33" s="14"/>
+      <c r="AW33" s="14"/>
+      <c r="AX33" s="14"/>
+      <c r="AY33" s="14"/>
+      <c r="AZ33" s="14"/>
+      <c r="BA33" s="14"/>
+    </row>
+    <row r="34" spans="31:53" x14ac:dyDescent="0.25">
       <c r="AE34" s="2">
         <v>1.4457656960493299</v>
       </c>
       <c r="AF34" s="2">
         <v>33.396957666669799</v>
       </c>
-      <c r="AQ34" s="8">
-        <v>-1.18723988828468</v>
-      </c>
-      <c r="AR34" s="8">
-        <v>-6.4016622895761204</v>
-      </c>
-      <c r="AS34" s="19"/>
-      <c r="AT34" s="8">
-        <v>-0.62541832057584101</v>
-      </c>
-      <c r="AU34" s="8">
-        <v>-2.9261873089532</v>
-      </c>
-      <c r="AV34" s="19"/>
-      <c r="AW34" s="19"/>
-      <c r="AX34" s="19"/>
-      <c r="AY34" s="19"/>
-      <c r="AZ34" s="19"/>
-      <c r="BA34" s="19"/>
-      <c r="BB34" s="19"/>
-      <c r="BC34" s="19"/>
-      <c r="BD34" s="19"/>
-    </row>
-    <row r="35" spans="31:56" x14ac:dyDescent="0.25">
+      <c r="AQ34">
+        <v>-5.0663103550460296</v>
+      </c>
+      <c r="AR34">
+        <v>3.1206464727475498</v>
+      </c>
+      <c r="AS34" s="14"/>
+      <c r="AT34" s="14"/>
+      <c r="AU34" s="14"/>
+      <c r="AV34" s="14"/>
+      <c r="AW34" s="14"/>
+      <c r="AX34" s="14"/>
+      <c r="AY34" s="14"/>
+      <c r="AZ34" s="14"/>
+      <c r="BA34" s="14"/>
+    </row>
+    <row r="35" spans="31:53" x14ac:dyDescent="0.25">
       <c r="AE35" s="2">
         <v>1.38172179023404</v>
       </c>
       <c r="AF35" s="2">
         <v>31.801475511643002</v>
       </c>
-      <c r="AQ35" s="8">
-        <v>-1.18635636607446</v>
-      </c>
-      <c r="AR35" s="8">
-        <v>-6.5579809851017199</v>
-      </c>
-      <c r="AS35" s="19"/>
-    </row>
-    <row r="36" spans="31:56" x14ac:dyDescent="0.25">
+      <c r="AQ35">
+        <v>-5.1335790936769996</v>
+      </c>
+      <c r="AR35">
+        <v>2.5614226667640598</v>
+      </c>
+    </row>
+    <row r="36" spans="31:53" x14ac:dyDescent="0.25">
       <c r="AE36" s="2">
         <v>1.5354675074703701</v>
       </c>
       <c r="AF36" s="2">
         <v>33.562475426831</v>
       </c>
-      <c r="AQ36" s="8">
-        <v>-1.0533089502570001</v>
-      </c>
-      <c r="AR36" s="8">
-        <v>-5.9093474102364603</v>
-      </c>
-    </row>
-    <row r="37" spans="31:56" x14ac:dyDescent="0.25">
+      <c r="AQ36" s="8"/>
+      <c r="AR36" s="8"/>
+    </row>
+    <row r="37" spans="31:53" x14ac:dyDescent="0.25">
       <c r="AE37" s="2">
         <v>1.4614764617699201</v>
       </c>
       <c r="AF37" s="2">
         <v>30.1235575379546</v>
       </c>
-      <c r="AQ37" s="8">
-        <v>-1.02273092988221</v>
-      </c>
-      <c r="AR37" s="8">
-        <v>-6.1893562181712101</v>
-      </c>
-    </row>
-    <row r="38" spans="31:56" x14ac:dyDescent="0.25">
+      <c r="AQ37" s="8"/>
+      <c r="AR37" s="8"/>
+    </row>
+    <row r="38" spans="31:53" x14ac:dyDescent="0.25">
       <c r="AE38" s="2">
         <v>1.59880330467955</v>
       </c>
       <c r="AF38" s="2">
         <v>29.9799133997208</v>
       </c>
-      <c r="AQ38" s="8">
-        <v>-0.98707595352328303</v>
-      </c>
-      <c r="AR38" s="8">
-        <v>-4.9885812023634299</v>
-      </c>
-    </row>
-    <row r="39" spans="31:56" x14ac:dyDescent="0.25">
+      <c r="AQ38" s="8"/>
+      <c r="AR38" s="8"/>
+    </row>
+    <row r="39" spans="31:53" x14ac:dyDescent="0.25">
       <c r="AE39" s="2">
         <v>1.6489991696386701</v>
       </c>
       <c r="AF39" s="2">
         <v>30.746215085486899</v>
       </c>
-      <c r="AQ39" s="8">
-        <v>-0.90262106045926604</v>
-      </c>
-      <c r="AR39" s="8">
-        <v>-5.3020187984014902</v>
-      </c>
-    </row>
-    <row r="40" spans="31:56" x14ac:dyDescent="0.25">
+      <c r="AQ39" s="8"/>
+      <c r="AR39" s="8"/>
+    </row>
+    <row r="40" spans="31:53" x14ac:dyDescent="0.25">
       <c r="AE40" s="2">
         <v>1.65675894733109</v>
       </c>
       <c r="AF40" s="2">
         <v>28.410402230959502</v>
       </c>
-      <c r="AQ40" s="8">
-        <v>-0.87187385682739604</v>
-      </c>
-      <c r="AR40" s="8">
-        <v>-4.4364154365608899</v>
-      </c>
-    </row>
-    <row r="41" spans="31:56" x14ac:dyDescent="0.25">
+      <c r="AQ40" s="8"/>
+      <c r="AR40" s="8"/>
+    </row>
+    <row r="41" spans="31:53" x14ac:dyDescent="0.25">
       <c r="AE41" s="2">
         <v>1.7544516698174499</v>
       </c>
       <c r="AF41" s="2">
         <v>27.930269926014901</v>
       </c>
-      <c r="AQ41" s="8">
-        <v>-0.77000988716855001</v>
-      </c>
-      <c r="AR41" s="8">
-        <v>-4.0551566171849096</v>
-      </c>
-    </row>
-    <row r="42" spans="31:56" x14ac:dyDescent="0.25">
+      <c r="AQ41" s="8"/>
+      <c r="AR41" s="8"/>
+    </row>
+    <row r="42" spans="31:53" x14ac:dyDescent="0.25">
       <c r="AE42" s="2">
         <v>1.8196302303724901</v>
       </c>
       <c r="AF42" s="2">
         <v>26.007077419416898</v>
       </c>
-      <c r="AQ42" s="8">
-        <v>-0.69278137820288799</v>
-      </c>
-      <c r="AR42" s="8">
-        <v>-3.5644466473455201</v>
-      </c>
-    </row>
-    <row r="43" spans="31:56" x14ac:dyDescent="0.25">
+      <c r="AQ42" s="8"/>
+      <c r="AR42" s="8"/>
+    </row>
+    <row r="43" spans="31:53" x14ac:dyDescent="0.25">
       <c r="AE43" s="2">
         <v>1.84298835891777</v>
       </c>
@@ -7898,123 +7663,101 @@
         <v>25.4837494388937</v>
       </c>
     </row>
-    <row r="52" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A52" s="14" t="s">
+    <row r="52" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A52" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
-      <c r="M52" s="14"/>
-      <c r="N52" s="14"/>
-      <c r="P52" s="14" t="s">
+      <c r="B52" s="16"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="16"/>
+      <c r="J52" s="16"/>
+      <c r="K52" s="16"/>
+      <c r="L52" s="16"/>
+      <c r="M52" s="16"/>
+      <c r="N52" s="16"/>
+      <c r="P52" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="Q52" s="14"/>
-      <c r="R52" s="14"/>
-      <c r="S52" s="14"/>
-      <c r="T52" s="14"/>
-      <c r="U52" s="14"/>
-      <c r="V52" s="14"/>
-      <c r="W52" s="14"/>
-      <c r="X52" s="14"/>
-      <c r="Y52" s="14"/>
-      <c r="Z52" s="14"/>
-      <c r="AA52" s="14"/>
-      <c r="AB52" s="14"/>
-      <c r="AC52" s="14"/>
-      <c r="AE52" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="AF52" s="14"/>
-      <c r="AG52" s="14"/>
-      <c r="AH52" s="14"/>
-      <c r="AI52" s="14"/>
-      <c r="AJ52" s="14"/>
-      <c r="AK52" s="14"/>
-      <c r="AL52" s="14"/>
-      <c r="AM52" s="14"/>
-      <c r="AN52" s="14"/>
-      <c r="AO52" s="14"/>
-      <c r="AQ52" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="AR52" s="14"/>
-      <c r="AS52" s="14"/>
-      <c r="AT52" s="14"/>
-      <c r="AU52" s="14"/>
-      <c r="AV52" s="14"/>
-      <c r="AW52" s="14"/>
-      <c r="AX52" s="14"/>
-      <c r="AY52" s="14"/>
-      <c r="AZ52" s="14"/>
-      <c r="BA52" s="14"/>
-      <c r="BB52" s="14"/>
-      <c r="BC52" s="14"/>
-      <c r="BD52" s="14"/>
-      <c r="BE52" s="14"/>
-      <c r="BF52" s="14"/>
-      <c r="BG52" s="14"/>
-    </row>
-    <row r="53" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="AE53" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="AF53" s="14"/>
-      <c r="AG53" s="14"/>
-      <c r="AH53" s="14"/>
-      <c r="AI53" s="14"/>
-      <c r="AJ53" s="14"/>
-      <c r="AK53" s="14"/>
-      <c r="AL53" s="14"/>
-      <c r="AM53" s="14"/>
-      <c r="AN53" s="14"/>
-      <c r="AO53" s="14"/>
-    </row>
-    <row r="54" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="AE54" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="AF54" s="14"/>
-      <c r="AG54" s="14"/>
-      <c r="AH54" s="14"/>
-      <c r="AI54" s="14"/>
-      <c r="AJ54" s="14"/>
-      <c r="AK54" s="14"/>
-      <c r="AL54" s="14"/>
-      <c r="AM54" s="14"/>
-      <c r="AN54" s="14"/>
-      <c r="AO54" s="14"/>
+      <c r="Q52" s="16"/>
+      <c r="R52" s="16"/>
+      <c r="S52" s="16"/>
+      <c r="T52" s="16"/>
+      <c r="U52" s="16"/>
+      <c r="V52" s="16"/>
+      <c r="W52" s="16"/>
+      <c r="X52" s="16"/>
+      <c r="Y52" s="16"/>
+      <c r="Z52" s="16"/>
+      <c r="AA52" s="16"/>
+      <c r="AB52" s="16"/>
+      <c r="AC52" s="16"/>
+      <c r="AE52" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF52" s="16"/>
+      <c r="AG52" s="16"/>
+      <c r="AH52" s="16"/>
+      <c r="AI52" s="16"/>
+      <c r="AJ52" s="16"/>
+      <c r="AK52" s="16"/>
+      <c r="AL52" s="16"/>
+      <c r="AM52" s="16"/>
+      <c r="AN52" s="16"/>
+      <c r="AO52" s="16"/>
+      <c r="AQ52" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="AR52" s="16"/>
+      <c r="AS52" s="16"/>
+      <c r="AT52" s="16"/>
+      <c r="AU52" s="16"/>
+      <c r="AV52" s="16"/>
+      <c r="AW52" s="16"/>
+      <c r="AX52" s="16"/>
+      <c r="AY52" s="16"/>
+      <c r="AZ52" s="16"/>
+      <c r="BA52" s="16"/>
+      <c r="BB52" s="16"/>
+      <c r="BC52" s="16"/>
+      <c r="BD52" s="16"/>
+    </row>
+    <row r="53" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="AE53" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF53" s="16"/>
+      <c r="AG53" s="16"/>
+      <c r="AH53" s="16"/>
+      <c r="AI53" s="16"/>
+      <c r="AJ53" s="16"/>
+      <c r="AK53" s="16"/>
+      <c r="AL53" s="16"/>
+      <c r="AM53" s="16"/>
+      <c r="AN53" s="16"/>
+      <c r="AO53" s="16"/>
+    </row>
+    <row r="54" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="AE54" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="AF54" s="16"/>
+      <c r="AG54" s="16"/>
+      <c r="AH54" s="16"/>
+      <c r="AI54" s="16"/>
+      <c r="AJ54" s="16"/>
+      <c r="AK54" s="16"/>
+      <c r="AL54" s="16"/>
+      <c r="AM54" s="16"/>
+      <c r="AN54" s="16"/>
+      <c r="AO54" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="AQ52:BG52"/>
-    <mergeCell ref="AQ1:AR1"/>
-    <mergeCell ref="AT1:AU1"/>
-    <mergeCell ref="AW1:AX1"/>
-    <mergeCell ref="AZ1:BA1"/>
-    <mergeCell ref="BF1:BG1"/>
-    <mergeCell ref="BC1:BD1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="P52:AC52"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="A52:N52"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="M1:N1"/>
+  <mergeCells count="25">
     <mergeCell ref="AE53:AO53"/>
     <mergeCell ref="AE52:AO52"/>
     <mergeCell ref="AE54:AO54"/>
@@ -8022,6 +7765,24 @@
     <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="AK1:AL1"/>
     <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="A52:N52"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="P52:AC52"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AQ52:BD52"/>
+    <mergeCell ref="AQ1:AR1"/>
+    <mergeCell ref="AT1:AU1"/>
+    <mergeCell ref="AW1:AX1"/>
+    <mergeCell ref="BC1:BD1"/>
+    <mergeCell ref="AZ1:BA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8033,8 +7794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A88C06-9205-4EF5-AC1B-94A0B27B9154}">
   <dimension ref="A1:AR51"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8062,66 +7823,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="D1" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="E1" s="14"/>
-      <c r="G1" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" s="14"/>
-      <c r="J1" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="K1" s="14"/>
-      <c r="M1" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="N1" s="14"/>
-      <c r="P1" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q1" s="14"/>
-      <c r="S1" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="T1" s="14"/>
-      <c r="V1" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="W1" s="14"/>
-      <c r="Y1" s="14" t="s">
+      <c r="A1" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="D1" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="16"/>
+      <c r="G1" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="J1" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="K1" s="16"/>
+      <c r="M1" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="N1" s="16"/>
+      <c r="P1" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q1" s="16"/>
+      <c r="S1" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="T1" s="16"/>
+      <c r="V1" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="W1" s="16"/>
+      <c r="Y1" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z1" s="16"/>
+      <c r="AB1" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC1" s="16"/>
+      <c r="AE1" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF1" s="16"/>
+      <c r="AH1" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI1" s="16"/>
+      <c r="AK1" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="AL1" s="16"/>
+      <c r="AN1" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="Z1" s="14"/>
-      <c r="AB1" s="14" t="s">
+      <c r="AO1" s="16"/>
+      <c r="AQ1" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="AC1" s="14"/>
-      <c r="AE1" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="AF1" s="14"/>
-      <c r="AH1" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI1" s="14"/>
-      <c r="AK1" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="AL1" s="14"/>
-      <c r="AN1" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="AO1" s="14"/>
-      <c r="AQ1" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="AR1" s="14"/>
+      <c r="AR1" s="16"/>
     </row>
     <row r="3" spans="1:44" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -8173,46 +7934,46 @@
         <v>58</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="AH3" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="AI3" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="AK3" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="AL3" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="AN3" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="AO3" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="AQ3" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="AR3" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
@@ -9192,90 +8953,89 @@
       </c>
     </row>
     <row r="40" spans="1:23" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="M40" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
-      <c r="P40" s="14"/>
-      <c r="Q40" s="14"/>
-      <c r="R40" s="14"/>
-      <c r="S40" s="14"/>
-      <c r="T40" s="14"/>
-      <c r="U40" s="14"/>
-      <c r="V40" s="14"/>
-      <c r="W40" s="14"/>
+      <c r="A40" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="M40" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="N40" s="16"/>
+      <c r="O40" s="16"/>
+      <c r="P40" s="16"/>
+      <c r="Q40" s="16"/>
+      <c r="R40" s="16"/>
+      <c r="S40" s="16"/>
+      <c r="T40" s="16"/>
+      <c r="U40" s="16"/>
+      <c r="V40" s="16"/>
+      <c r="W40" s="16"/>
     </row>
     <row r="49" spans="25:44" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Y49" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z49" s="14"/>
-      <c r="AA49" s="14"/>
-      <c r="AB49" s="14"/>
-      <c r="AC49" s="14"/>
-      <c r="AD49" s="14"/>
-      <c r="AE49" s="14"/>
-      <c r="AF49" s="14"/>
-      <c r="AH49" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="AI49" s="14"/>
-      <c r="AJ49" s="14"/>
-      <c r="AK49" s="14"/>
-      <c r="AL49" s="14"/>
-      <c r="AM49" s="14"/>
-      <c r="AN49" s="14"/>
-      <c r="AO49" s="14"/>
-      <c r="AP49" s="14"/>
-      <c r="AQ49" s="14"/>
-      <c r="AR49" s="14"/>
+      <c r="Y49" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z49" s="16"/>
+      <c r="AA49" s="16"/>
+      <c r="AB49" s="16"/>
+      <c r="AC49" s="16"/>
+      <c r="AD49" s="16"/>
+      <c r="AE49" s="16"/>
+      <c r="AF49" s="16"/>
+      <c r="AH49" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI49" s="16"/>
+      <c r="AJ49" s="16"/>
+      <c r="AK49" s="16"/>
+      <c r="AL49" s="16"/>
+      <c r="AM49" s="16"/>
+      <c r="AN49" s="16"/>
+      <c r="AO49" s="16"/>
+      <c r="AP49" s="16"/>
+      <c r="AQ49" s="16"/>
+      <c r="AR49" s="16"/>
     </row>
     <row r="50" spans="25:44" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Y50" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="Z50" s="14"/>
-      <c r="AA50" s="14"/>
-      <c r="AB50" s="14"/>
-      <c r="AC50" s="14"/>
-      <c r="AD50" s="14"/>
-      <c r="AE50" s="14"/>
-      <c r="AF50" s="14"/>
+      <c r="Y50" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z50" s="16"/>
+      <c r="AA50" s="16"/>
+      <c r="AB50" s="16"/>
+      <c r="AC50" s="16"/>
+      <c r="AD50" s="16"/>
+      <c r="AE50" s="16"/>
+      <c r="AF50" s="16"/>
     </row>
     <row r="51" spans="25:44" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Y51" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="Z51" s="14"/>
-      <c r="AA51" s="14"/>
-      <c r="AB51" s="14"/>
-      <c r="AC51" s="14"/>
-      <c r="AD51" s="14"/>
-      <c r="AE51" s="14"/>
-      <c r="AF51" s="14"/>
+      <c r="Y51" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z51" s="16"/>
+      <c r="AA51" s="16"/>
+      <c r="AB51" s="16"/>
+      <c r="AC51" s="16"/>
+      <c r="AD51" s="16"/>
+      <c r="AE51" s="16"/>
+      <c r="AF51" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="Y50:AF50"/>
-    <mergeCell ref="Y51:AF51"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="Y49:AF49"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AQ1:AR1"/>
+    <mergeCell ref="AH49:AR49"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="V1:W1"/>
@@ -9286,11 +9046,12 @@
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A40:K40"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="AQ1:AR1"/>
-    <mergeCell ref="AH49:AR49"/>
+    <mergeCell ref="Y50:AF50"/>
+    <mergeCell ref="Y51:AF51"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="Y49:AF49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9330,22 +9091,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="D1" s="13" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="G1" s="13" t="s">
+      <c r="E1" s="15"/>
+      <c r="G1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="J1" s="13" t="s">
+      <c r="H1" s="15"/>
+      <c r="J1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="13"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="3" spans="1:11" ht="61.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -9629,19 +9390,19 @@
       <c r="A38" s="9"/>
     </row>
     <row r="41" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
+      <c r="A41" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -9673,17 +9434,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="16"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -9863,10 +9624,10 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="177.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B38" s="15"/>
+      <c r="A38" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="17"/>
       <c r="H38" s="10"/>
     </row>
   </sheetData>
@@ -9905,67 +9666,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="D1" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="E1" s="14"/>
-      <c r="G1" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="14"/>
-      <c r="J1" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="K1" s="14"/>
-      <c r="M1" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="N1" s="14"/>
-      <c r="P1" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q1" s="14"/>
+      <c r="A1" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="D1" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="16"/>
+      <c r="G1" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="J1" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="16"/>
+      <c r="M1" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="16"/>
+      <c r="P1" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q1" s="16"/>
     </row>
     <row r="3" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -10425,25 +10186,25 @@
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-      <c r="Q38" s="14"/>
+      <c r="A38" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="16"/>
     </row>
     <row r="52" ht="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -10484,18 +10245,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="D1" s="13" t="s">
+      <c r="B1" s="15"/>
+      <c r="D1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="G1" s="13" t="s">
+      <c r="E1" s="15"/>
+      <c r="G1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="13"/>
+      <c r="H1" s="15"/>
     </row>
     <row r="3" spans="1:8" ht="46.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -11075,13 +10836,13 @@
     </row>
     <row r="59" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="68" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="14" t="s">
+      <c r="A68" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B68" s="14"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="14"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -11109,10 +10870,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="16"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -11151,10 +10912,10 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="14"/>
+      <c r="B25" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -11192,34 +10953,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="D1" s="14" t="s">
+      <c r="B1" s="16"/>
+      <c r="D1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="G1" s="14" t="s">
+      <c r="E1" s="16"/>
+      <c r="G1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="J1" s="14" t="s">
+      <c r="H1" s="16"/>
+      <c r="J1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="M1" s="14" t="s">
+      <c r="K1" s="16"/>
+      <c r="M1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="14"/>
-      <c r="P1" s="14" t="s">
+      <c r="N1" s="16"/>
+      <c r="P1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="14"/>
-      <c r="S1" s="14" t="s">
+      <c r="Q1" s="16"/>
+      <c r="S1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="14"/>
+      <c r="T1" s="16"/>
     </row>
     <row r="3" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -11664,28 +11425,28 @@
       <c r="A34" s="7"/>
     </row>
     <row r="38" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="N38" s="14"/>
-      <c r="O38" s="14"/>
-      <c r="P38" s="14"/>
-      <c r="Q38" s="14"/>
-      <c r="R38" s="14"/>
-      <c r="S38" s="14"/>
-      <c r="T38" s="14"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="16"/>
+      <c r="S38" s="16"/>
+      <c r="T38" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -11750,10 +11511,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="16"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -11808,10 +11569,10 @@
       </c>
     </row>
     <row r="29" spans="1:2" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="14"/>
+      <c r="B29" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>